<commit_message>
add comparision of w2v models
</commit_message>
<xml_diff>
--- a/results/Display Results.xlsx
+++ b/results/Display Results.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garim\Downloads\Portfolio_ML\emotional_classification\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454D0D49-7514-44B1-9C1F-5576B74ACF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8106446-8B2F-4733-8172-53BF26B76130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" xr2:uid="{71182A3D-F6EC-4B17-9398-B1568EC59A44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" activeTab="1" xr2:uid="{71182A3D-F6EC-4B17-9398-B1568EC59A44}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TFIDF Compare" sheetId="1" r:id="rId1"/>
+    <sheet name="Word2Vec Compare" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Multinomial
 Naïve Bayes</t>
@@ -72,12 +74,21 @@
   <si>
     <t>Accuracy</t>
   </si>
+  <si>
+    <t>Custom Model</t>
+  </si>
+  <si>
+    <t>Google News Model</t>
+  </si>
+  <si>
+    <t>Words Most Similar to 'Affectionate'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +130,27 @@
     <font>
       <sz val="13"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.5"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,11 +251,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -235,12 +273,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,6 +559,163 @@
           </cell>
           <cell r="F10" t="str">
             <v>0.8627759913794953</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="w2v_simlarity_affectionate"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>compassionate</v>
+          </cell>
+          <cell r="C2">
+            <v>0.95496189594268799</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>playful</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>0.6595738530158997</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>hateful</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>0.9520337581634521</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>loving</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>0.6079658269882202</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>submissive</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>0.9467794895172119</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>endearing</v>
+          </cell>
+          <cell r="E4" t="str">
+            <v>0.6056519746780396</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>considerate</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>0.9441692233085632</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>affection</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>0.5745200514793396</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>hostile</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>0.9406910538673401</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>flirtatious</v>
+          </cell>
+          <cell r="E6">
+            <v>0.55764240026473999</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>unfriendly</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>0.9368013143539429</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>lovable</v>
+          </cell>
+          <cell r="E7" t="str">
+            <v>0.5493666529655457</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>truthful</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>0.9362722635269165</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>gentle</v>
+          </cell>
+          <cell r="E8" t="str">
+            <v>0.5466917753219604</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>sympathetic</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>0.9343375563621521</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>sociable</v>
+          </cell>
+          <cell r="E9">
+            <v>0.5462646484375</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>insincere</v>
+          </cell>
+          <cell r="C10">
+            <v>0.929573655128479</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>good_natured</v>
+          </cell>
+          <cell r="E10" t="str">
+            <v>0.5455296039581299</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>victimized</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>0.9248496890068054</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>charming</v>
+          </cell>
+          <cell r="E11" t="str">
+            <v>0.5257826447486877</v>
           </cell>
         </row>
       </sheetData>
@@ -839,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90C2A2B-A7A6-482D-B758-9D20D0D31763}">
   <dimension ref="B5:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -872,261 +1076,261 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="str">
+      <c r="C6" s="7" t="str">
         <f>[1]tfidf_results!A2</f>
         <v>anger</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B2)</f>
         <v>0.79885767212102499</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C2)</f>
         <v>0.84902747761654795</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D2)</f>
         <v>0.82630441494288298</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E2)</f>
         <v>0.81404754553874603</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F2)</f>
         <v>0.82973139857980804</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8" t="str">
+      <c r="B7" s="10"/>
+      <c r="C7" s="7" t="str">
         <f>[1]tfidf_results!A3</f>
         <v>fear</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B3)</f>
         <v>0.75090121254050901</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C3)</f>
         <v>0.80675818373812003</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D3)</f>
         <v>0.82321669154862898</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E3)</f>
         <v>0.83406765466263699</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F3)</f>
         <v>0.82915194989622398</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8" t="str">
+      <c r="B8" s="10"/>
+      <c r="C8" s="7" t="str">
         <f>[1]tfidf_results!A4</f>
         <v>joy</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B4)</f>
         <v>0.96708663827182495</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C4)</f>
         <v>0.94125073325001896</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D4)</f>
         <v>0.96002193373970202</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E4)</f>
         <v>0.92098752837358699</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F4)</f>
         <v>0.93053890688362295</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="str">
+      <c r="B9" s="10"/>
+      <c r="C9" s="7" t="str">
         <f>[1]tfidf_results!A5</f>
         <v>love</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B5)</f>
         <v>0.555497051390059</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C5)</f>
         <v>0.75842459983150801</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D5)</f>
         <v>0.69002737994945196</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E5)</f>
         <v>0.67965459140690798</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F5)</f>
         <v>0.66312131423757303</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8" t="str">
+      <c r="B10" s="10"/>
+      <c r="C10" s="7" t="str">
         <f>[1]tfidf_results!A6</f>
         <v>sadness</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B6)</f>
         <v>0.94311727983154603</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C6)</f>
         <v>0.92805136646054798</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D6)</f>
         <v>0.92659815828106196</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E6)</f>
         <v>0.88623455966309295</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F6)</f>
         <v>0.89903168883550499</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8" t="str">
+      <c r="B11" s="10"/>
+      <c r="C11" s="7" t="str">
         <f>[1]tfidf_results!A7</f>
         <v>surprise</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B7)</f>
         <v>0.42402526418073599</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C7)</f>
         <v>0.72585934653224804</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D7)</f>
         <v>0.65504676302684295</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E7)</f>
         <v>0.61994412729260295</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F7)</f>
         <v>0.62310214988460999</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B8)</f>
         <v>0.858512962955012</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C8)</f>
         <v>0.88622908733412598</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D8)</f>
         <v>0.88282896798650201</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E8)</f>
         <v>0.85549063464601405</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F8)</f>
         <v>0.86277599137949501</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B9)</f>
         <v>0.73991418638928297</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C9)</f>
         <v>0.83489528457149798</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D9)</f>
         <v>0.81353589024809503</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E9)</f>
         <v>0.79248933448959502</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F9)</f>
         <v>0.79577956805289096</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="2:8" ht="17" x14ac:dyDescent="0.4">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14">
+      <c r="C16" s="11"/>
+      <c r="D16" s="9">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B10)</f>
         <v>0.858512962955012</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="9">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!C10)</f>
         <v>0.88622908733412598</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="9">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!D10)</f>
         <v>0.88282896798650201</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="9">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!E10)</f>
         <v>0.85549063464601405</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="9">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!F10)</f>
         <v>0.86277599137949501</v>
       </c>
@@ -1169,4 +1373,242 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66472120-7198-4781-AF1D-D899A06886A7}">
+  <dimension ref="E7:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="15.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="5:8" ht="16.5" x14ac:dyDescent="0.4">
+      <c r="E7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E9" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!B2</f>
+        <v>compassionate</v>
+      </c>
+      <c r="F9" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C2)</f>
+        <v>0.95496189594268799</v>
+      </c>
+      <c r="G9" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D2</f>
+        <v>playful</v>
+      </c>
+      <c r="H9" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E2)</f>
+        <v>0.65957385301589899</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E10" s="20" t="str">
+        <f>[2]w2v_simlarity_affectionate!B3</f>
+        <v>hateful</v>
+      </c>
+      <c r="F10" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C3)</f>
+        <v>0.95203375816345204</v>
+      </c>
+      <c r="G10" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D3</f>
+        <v>loving</v>
+      </c>
+      <c r="H10" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E3)</f>
+        <v>0.60796582698821999</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E11" s="20" t="str">
+        <f>[2]w2v_simlarity_affectionate!B4</f>
+        <v>submissive</v>
+      </c>
+      <c r="F11" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C4)</f>
+        <v>0.94677948951721103</v>
+      </c>
+      <c r="G11" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D4</f>
+        <v>endearing</v>
+      </c>
+      <c r="H11" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E4)</f>
+        <v>0.605651974678039</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E12" s="21" t="str">
+        <f>[2]w2v_simlarity_affectionate!B5</f>
+        <v>considerate</v>
+      </c>
+      <c r="F12" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C5)</f>
+        <v>0.94416922330856301</v>
+      </c>
+      <c r="G12" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D5</f>
+        <v>affection</v>
+      </c>
+      <c r="H12" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E5)</f>
+        <v>0.57452005147933904</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E13" s="20" t="str">
+        <f>[2]w2v_simlarity_affectionate!B6</f>
+        <v>hostile</v>
+      </c>
+      <c r="F13" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C6)</f>
+        <v>0.94069105386733998</v>
+      </c>
+      <c r="G13" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D6</f>
+        <v>flirtatious</v>
+      </c>
+      <c r="H13" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E6)</f>
+        <v>0.55764240026473999</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E14" s="20" t="str">
+        <f>[2]w2v_simlarity_affectionate!B7</f>
+        <v>unfriendly</v>
+      </c>
+      <c r="F14" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C7)</f>
+        <v>0.93680131435394198</v>
+      </c>
+      <c r="G14" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D7</f>
+        <v>lovable</v>
+      </c>
+      <c r="H14" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E7)</f>
+        <v>0.54936665296554499</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E15" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!B8</f>
+        <v>truthful</v>
+      </c>
+      <c r="F15" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C8)</f>
+        <v>0.93627226352691595</v>
+      </c>
+      <c r="G15" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D8</f>
+        <v>gentle</v>
+      </c>
+      <c r="H15" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E8)</f>
+        <v>0.54669177532196001</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E16" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!B9</f>
+        <v>sympathetic</v>
+      </c>
+      <c r="F16" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C9)</f>
+        <v>0.93433755636215199</v>
+      </c>
+      <c r="G16" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D9</f>
+        <v>sociable</v>
+      </c>
+      <c r="H16" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E9)</f>
+        <v>0.5462646484375</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E17" s="20" t="str">
+        <f>[2]w2v_simlarity_affectionate!B10</f>
+        <v>insincere</v>
+      </c>
+      <c r="F17" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C10)</f>
+        <v>0.929573655128479</v>
+      </c>
+      <c r="G17" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D10</f>
+        <v>good_natured</v>
+      </c>
+      <c r="H17" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E10)</f>
+        <v>0.54552960395812899</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E18" s="20" t="str">
+        <f>[2]w2v_simlarity_affectionate!B11</f>
+        <v>victimized</v>
+      </c>
+      <c r="F18" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C11)</f>
+        <v>0.92484968900680498</v>
+      </c>
+      <c r="G18" s="18" t="str">
+        <f>[2]w2v_simlarity_affectionate!D11</f>
+        <v>charming</v>
+      </c>
+      <c r="H18" s="19">
+        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E11)</f>
+        <v>0.52578264474868697</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E7:H7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F9:H18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edit text in the WordVec readme portion. compare TF-IDF classification to word2vec
</commit_message>
<xml_diff>
--- a/results/Display Results.xlsx
+++ b/results/Display Results.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garim\Downloads\Portfolio_ML\emotional_classification\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8106446-8B2F-4733-8172-53BF26B76130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A595052-961D-4A74-A5E3-6A294A7E7196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" activeTab="1" xr2:uid="{71182A3D-F6EC-4B17-9398-B1568EC59A44}"/>
   </bookViews>
   <sheets>
     <sheet name="TFIDF Compare" sheetId="1" r:id="rId1"/>
-    <sheet name="Word2Vec Compare" sheetId="2" r:id="rId2"/>
+    <sheet name="TFIDF W2V Compare" sheetId="3" r:id="rId2"/>
+    <sheet name="Word2Vec Compare" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Multinomial
 Naïve Bayes</t>
@@ -82,6 +84,17 @@
   </si>
   <si>
     <t>Words Most Similar to 'Affectionate'</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Word2Vec
+Embeddings</t>
+  </si>
+  <si>
+    <t>TF-IDF 
+Vectorizer</t>
   </si>
 </sst>
 </file>
@@ -170,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -230,12 +243,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -288,6 +310,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,6 +747,95 @@
           </cell>
           <cell r="E11" t="str">
             <v>0.5257826447486877</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="w2v_results"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2">
+            <v>0.58701890946259305</v>
+          </cell>
+          <cell r="C2">
+            <v>0.56323465817509899</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>0.56055267062314496</v>
+          </cell>
+          <cell r="C3">
+            <v>0.54900778931750704</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>0.84596898595437198</v>
+          </cell>
+          <cell r="C4">
+            <v>0.83239425184703997</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>0.22257978010190399</v>
+          </cell>
+          <cell r="C5">
+            <v>0.33467417538214</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0.73867562923660801</v>
+          </cell>
+          <cell r="C6">
+            <v>0.75984214799569405</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>0.34642746674914898</v>
+          </cell>
+          <cell r="C7">
+            <v>0.37364676770801097</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>0.67676143724751603</v>
+          </cell>
+          <cell r="C8">
+            <v>0.68375306806317004</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>0.55020390702129496</v>
+          </cell>
+          <cell r="C9">
+            <v>0.56879996507091501</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>0.67676143724751603</v>
+          </cell>
+          <cell r="C10">
+            <v>0.68375306806317004</v>
           </cell>
         </row>
       </sheetData>
@@ -1376,11 +1496,445 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543AA1EA-9BC7-4F6A-918E-A30F4C4A2D04}">
+  <dimension ref="B4:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="5.08984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="4" customWidth="1"/>
+    <col min="4" max="8" width="12.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="1.453125" style="2" customWidth="1"/>
+    <col min="10" max="11" width="12.26953125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11" s="24" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D4" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="J4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="22"/>
+    </row>
+    <row r="5" spans="2:11" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f>[1]tfidf_results!A2</f>
+        <v>anger</v>
+      </c>
+      <c r="D6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B2)</f>
+        <v>0.79885767212102499</v>
+      </c>
+      <c r="E6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C2)</f>
+        <v>0.84902747761654795</v>
+      </c>
+      <c r="F6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D2)</f>
+        <v>0.82630441494288298</v>
+      </c>
+      <c r="G6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E2)</f>
+        <v>0.81404754553874603</v>
+      </c>
+      <c r="H6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F2)</f>
+        <v>0.82973139857980804</v>
+      </c>
+      <c r="J6" s="8">
+        <f>[3]w2v_results!C2</f>
+        <v>0.56323465817509899</v>
+      </c>
+      <c r="K6" s="8">
+        <f>[3]w2v_results!B2</f>
+        <v>0.58701890946259305</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="10"/>
+      <c r="C7" s="7" t="str">
+        <f>[1]tfidf_results!A3</f>
+        <v>fear</v>
+      </c>
+      <c r="D7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B3)</f>
+        <v>0.75090121254050901</v>
+      </c>
+      <c r="E7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C3)</f>
+        <v>0.80675818373812003</v>
+      </c>
+      <c r="F7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D3)</f>
+        <v>0.82321669154862898</v>
+      </c>
+      <c r="G7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E3)</f>
+        <v>0.83406765466263699</v>
+      </c>
+      <c r="H7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F3)</f>
+        <v>0.82915194989622398</v>
+      </c>
+      <c r="J7" s="8">
+        <f>[3]w2v_results!C3</f>
+        <v>0.54900778931750704</v>
+      </c>
+      <c r="K7" s="8">
+        <f>[3]w2v_results!B3</f>
+        <v>0.56055267062314496</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B8" s="10"/>
+      <c r="C8" s="7" t="str">
+        <f>[1]tfidf_results!A4</f>
+        <v>joy</v>
+      </c>
+      <c r="D8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B4)</f>
+        <v>0.96708663827182495</v>
+      </c>
+      <c r="E8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C4)</f>
+        <v>0.94125073325001896</v>
+      </c>
+      <c r="F8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D4)</f>
+        <v>0.96002193373970202</v>
+      </c>
+      <c r="G8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E4)</f>
+        <v>0.92098752837358699</v>
+      </c>
+      <c r="H8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F4)</f>
+        <v>0.93053890688362295</v>
+      </c>
+      <c r="J8" s="8">
+        <f>[3]w2v_results!C4</f>
+        <v>0.83239425184703997</v>
+      </c>
+      <c r="K8" s="8">
+        <f>[3]w2v_results!B4</f>
+        <v>0.84596898595437198</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B9" s="10"/>
+      <c r="C9" s="7" t="str">
+        <f>[1]tfidf_results!A5</f>
+        <v>love</v>
+      </c>
+      <c r="D9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B5)</f>
+        <v>0.555497051390059</v>
+      </c>
+      <c r="E9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C5)</f>
+        <v>0.75842459983150801</v>
+      </c>
+      <c r="F9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D5)</f>
+        <v>0.69002737994945196</v>
+      </c>
+      <c r="G9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E5)</f>
+        <v>0.67965459140690798</v>
+      </c>
+      <c r="H9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F5)</f>
+        <v>0.66312131423757303</v>
+      </c>
+      <c r="J9" s="8">
+        <f>[3]w2v_results!C5</f>
+        <v>0.33467417538214</v>
+      </c>
+      <c r="K9" s="8">
+        <f>[3]w2v_results!B5</f>
+        <v>0.22257978010190399</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B10" s="10"/>
+      <c r="C10" s="7" t="str">
+        <f>[1]tfidf_results!A6</f>
+        <v>sadness</v>
+      </c>
+      <c r="D10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B6)</f>
+        <v>0.94311727983154603</v>
+      </c>
+      <c r="E10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C6)</f>
+        <v>0.92805136646054798</v>
+      </c>
+      <c r="F10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D6)</f>
+        <v>0.92659815828106196</v>
+      </c>
+      <c r="G10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E6)</f>
+        <v>0.88623455966309295</v>
+      </c>
+      <c r="H10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F6)</f>
+        <v>0.89903168883550499</v>
+      </c>
+      <c r="J10" s="8">
+        <f>[3]w2v_results!C6</f>
+        <v>0.75984214799569405</v>
+      </c>
+      <c r="K10" s="8">
+        <f>[3]w2v_results!B6</f>
+        <v>0.73867562923660801</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B11" s="10"/>
+      <c r="C11" s="7" t="str">
+        <f>[1]tfidf_results!A7</f>
+        <v>surprise</v>
+      </c>
+      <c r="D11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B7)</f>
+        <v>0.42402526418073599</v>
+      </c>
+      <c r="E11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C7)</f>
+        <v>0.72585934653224804</v>
+      </c>
+      <c r="F11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D7)</f>
+        <v>0.65504676302684295</v>
+      </c>
+      <c r="G11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E7)</f>
+        <v>0.61994412729260295</v>
+      </c>
+      <c r="H11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F7)</f>
+        <v>0.62310214988460999</v>
+      </c>
+      <c r="J11" s="8">
+        <f>[3]w2v_results!C7</f>
+        <v>0.37364676770801097</v>
+      </c>
+      <c r="K11" s="8">
+        <f>[3]w2v_results!B7</f>
+        <v>0.34642746674914898</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="10"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="10"/>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B8)</f>
+        <v>0.858512962955012</v>
+      </c>
+      <c r="E13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C8)</f>
+        <v>0.88622908733412598</v>
+      </c>
+      <c r="F13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D8)</f>
+        <v>0.88282896798650201</v>
+      </c>
+      <c r="G13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E8)</f>
+        <v>0.85549063464601405</v>
+      </c>
+      <c r="H13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F8)</f>
+        <v>0.86277599137949501</v>
+      </c>
+      <c r="J13" s="8">
+        <f>[3]w2v_results!C8</f>
+        <v>0.68375306806317004</v>
+      </c>
+      <c r="K13" s="8">
+        <f>[3]w2v_results!B8</f>
+        <v>0.67676143724751603</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="10"/>
+      <c r="C14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B9)</f>
+        <v>0.73991418638928297</v>
+      </c>
+      <c r="E14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C9)</f>
+        <v>0.83489528457149798</v>
+      </c>
+      <c r="F14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D9)</f>
+        <v>0.81353589024809503</v>
+      </c>
+      <c r="G14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E9)</f>
+        <v>0.79248933448959502</v>
+      </c>
+      <c r="H14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F9)</f>
+        <v>0.79577956805289096</v>
+      </c>
+      <c r="J14" s="8">
+        <f>[3]w2v_results!C9</f>
+        <v>0.56879996507091501</v>
+      </c>
+      <c r="K14" s="8">
+        <f>[3]w2v_results!B9</f>
+        <v>0.55020390702129496</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="2:11" ht="17" x14ac:dyDescent="0.4">
+      <c r="B16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B10)</f>
+        <v>0.858512962955012</v>
+      </c>
+      <c r="E16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C10)</f>
+        <v>0.88622908733412598</v>
+      </c>
+      <c r="F16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D10)</f>
+        <v>0.88282896798650201</v>
+      </c>
+      <c r="G16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E10)</f>
+        <v>0.85549063464601405</v>
+      </c>
+      <c r="H16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F10)</f>
+        <v>0.86277599137949501</v>
+      </c>
+      <c r="J16" s="9">
+        <f>[3]w2v_results!C10</f>
+        <v>0.68375306806317004</v>
+      </c>
+      <c r="K16" s="9">
+        <f>[3]w2v_results!B10</f>
+        <v>0.67676143724751603</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="J4:K4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6:K14">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:K16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0.84"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66472120-7198-4781-AF1D-D899A06886A7}">
   <dimension ref="E7:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
download BERT chart and scores and add to Readme
</commit_message>
<xml_diff>
--- a/results/Display Results.xlsx
+++ b/results/Display Results.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garim\Downloads\Portfolio_ML\emotional_classification\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A595052-961D-4A74-A5E3-6A294A7E7196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6224E6AD-110B-4209-9851-A8133DB9CEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" activeTab="1" xr2:uid="{71182A3D-F6EC-4B17-9398-B1568EC59A44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" activeTab="2" xr2:uid="{71182A3D-F6EC-4B17-9398-B1568EC59A44}"/>
   </bookViews>
   <sheets>
     <sheet name="TFIDF Compare" sheetId="1" r:id="rId1"/>
-    <sheet name="TFIDF W2V Compare" sheetId="3" r:id="rId2"/>
-    <sheet name="Word2Vec Compare" sheetId="2" r:id="rId3"/>
+    <sheet name="TFIDF W2V Compare" sheetId="5" r:id="rId2"/>
+    <sheet name="TFIDF W2V BERT Compare" sheetId="3" r:id="rId3"/>
+    <sheet name="Google vs Custom W2V Similarity" sheetId="2" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>Multinomial
 Naïve Bayes</t>
@@ -95,6 +97,12 @@
   <si>
     <t>TF-IDF 
 Vectorizer</t>
+  </si>
+  <si>
+    <t>BERT Embeddings</t>
+  </si>
+  <si>
+    <t>Neural Network Classifier</t>
   </si>
 </sst>
 </file>
@@ -257,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -280,6 +288,21 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -295,28 +318,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -410,6 +421,79 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FCF4F69-52BA-4F82-8F21-E44C39462B42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7893050" y="698500"/>
+          <a:ext cx="1111250" cy="2997200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -605,148 +689,80 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="w2v_simlarity_affectionate"/>
+      <sheetName val="w2v_results"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0" refreshError="1">
         <row r="2">
-          <cell r="B2" t="str">
-            <v>compassionate</v>
+          <cell r="B2">
+            <v>0.58701890946259305</v>
           </cell>
           <cell r="C2">
-            <v>0.95496189594268799</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>playful</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>0.6595738530158997</v>
+            <v>0.56323465817509899</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="B3" t="str">
-            <v>hateful</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>0.9520337581634521</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>loving</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v>0.6079658269882202</v>
+          <cell r="B3">
+            <v>0.56055267062314496</v>
+          </cell>
+          <cell r="C3">
+            <v>0.54900778931750704</v>
           </cell>
         </row>
         <row r="4">
-          <cell r="B4" t="str">
-            <v>submissive</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>0.9467794895172119</v>
-          </cell>
-          <cell r="D4" t="str">
-            <v>endearing</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>0.6056519746780396</v>
+          <cell r="B4">
+            <v>0.84596898595437198</v>
+          </cell>
+          <cell r="C4">
+            <v>0.83239425184703997</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="B5" t="str">
-            <v>considerate</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>0.9441692233085632</v>
-          </cell>
-          <cell r="D5" t="str">
-            <v>affection</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>0.5745200514793396</v>
+          <cell r="B5">
+            <v>0.22257978010190399</v>
+          </cell>
+          <cell r="C5">
+            <v>0.33467417538214</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="B6" t="str">
-            <v>hostile</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>0.9406910538673401</v>
-          </cell>
-          <cell r="D6" t="str">
-            <v>flirtatious</v>
-          </cell>
-          <cell r="E6">
-            <v>0.55764240026473999</v>
+          <cell r="B6">
+            <v>0.73867562923660801</v>
+          </cell>
+          <cell r="C6">
+            <v>0.75984214799569405</v>
           </cell>
         </row>
         <row r="7">
-          <cell r="B7" t="str">
-            <v>unfriendly</v>
-          </cell>
-          <cell r="C7" t="str">
-            <v>0.9368013143539429</v>
-          </cell>
-          <cell r="D7" t="str">
-            <v>lovable</v>
-          </cell>
-          <cell r="E7" t="str">
-            <v>0.5493666529655457</v>
+          <cell r="B7">
+            <v>0.34642746674914898</v>
+          </cell>
+          <cell r="C7">
+            <v>0.37364676770801097</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="B8" t="str">
-            <v>truthful</v>
-          </cell>
-          <cell r="C8" t="str">
-            <v>0.9362722635269165</v>
-          </cell>
-          <cell r="D8" t="str">
-            <v>gentle</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>0.5466917753219604</v>
+          <cell r="B8">
+            <v>0.67676143724751603</v>
+          </cell>
+          <cell r="C8">
+            <v>0.68375306806317004</v>
           </cell>
         </row>
         <row r="9">
-          <cell r="B9" t="str">
-            <v>sympathetic</v>
-          </cell>
-          <cell r="C9" t="str">
-            <v>0.9343375563621521</v>
-          </cell>
-          <cell r="D9" t="str">
-            <v>sociable</v>
-          </cell>
-          <cell r="E9">
-            <v>0.5462646484375</v>
+          <cell r="B9">
+            <v>0.55020390702129496</v>
+          </cell>
+          <cell r="C9">
+            <v>0.56879996507091501</v>
           </cell>
         </row>
         <row r="10">
-          <cell r="B10" t="str">
-            <v>insincere</v>
+          <cell r="B10">
+            <v>0.67676143724751603</v>
           </cell>
           <cell r="C10">
-            <v>0.929573655128479</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>good_natured</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>0.5455296039581299</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>victimized</v>
-          </cell>
-          <cell r="C11" t="str">
-            <v>0.9248496890068054</v>
-          </cell>
-          <cell r="D11" t="str">
-            <v>charming</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>0.5257826447486877</v>
+            <v>0.68375306806317004</v>
           </cell>
         </row>
       </sheetData>
@@ -762,80 +778,210 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="w2v_results"/>
+      <sheetName val="w2v_simlarity_affectionate"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>compassionate</v>
+          </cell>
+          <cell r="C2">
+            <v>0.95496189594268799</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>playful</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>0.6595738530158997</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>hateful</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>0.9520337581634521</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>loving</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>0.6079658269882202</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>submissive</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>0.9467794895172119</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>endearing</v>
+          </cell>
+          <cell r="E4" t="str">
+            <v>0.6056519746780396</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>considerate</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>0.9441692233085632</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>affection</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>0.5745200514793396</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>hostile</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>0.9406910538673401</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>flirtatious</v>
+          </cell>
+          <cell r="E6">
+            <v>0.55764240026473999</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>unfriendly</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>0.9368013143539429</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>lovable</v>
+          </cell>
+          <cell r="E7" t="str">
+            <v>0.5493666529655457</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>truthful</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>0.9362722635269165</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>gentle</v>
+          </cell>
+          <cell r="E8" t="str">
+            <v>0.5466917753219604</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>sympathetic</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>0.9343375563621521</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>sociable</v>
+          </cell>
+          <cell r="E9">
+            <v>0.5462646484375</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>insincere</v>
+          </cell>
+          <cell r="C10">
+            <v>0.929573655128479</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>good_natured</v>
+          </cell>
+          <cell r="E10" t="str">
+            <v>0.5455296039581299</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>victimized</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>0.9248496890068054</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>charming</v>
+          </cell>
+          <cell r="E11" t="str">
+            <v>0.5257826447486877</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="bert_results"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0.58701890946259305</v>
-          </cell>
-          <cell r="C2">
-            <v>0.56323465817509899</v>
+            <v>0.90571163939487498</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.56055267062314496</v>
-          </cell>
-          <cell r="C3">
-            <v>0.54900778931750704</v>
+            <v>0.89946473436987895</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>0.84596898595437198</v>
-          </cell>
-          <cell r="C4">
-            <v>0.83239425184703997</v>
+            <v>0.93714453314290003</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5">
-            <v>0.22257978010190399</v>
-          </cell>
-          <cell r="C5">
-            <v>0.33467417538214</v>
+            <v>0.87937026116259398</v>
           </cell>
         </row>
         <row r="6">
           <cell r="B6">
-            <v>0.73867562923660801</v>
-          </cell>
-          <cell r="C6">
-            <v>0.75984214799569405</v>
+            <v>0.98662455328677101</v>
           </cell>
         </row>
         <row r="7">
           <cell r="B7">
-            <v>0.34642746674914898</v>
-          </cell>
-          <cell r="C7">
-            <v>0.37364676770801097</v>
+            <v>0.80881817077614404</v>
           </cell>
         </row>
         <row r="8">
           <cell r="B8">
-            <v>0.67676143724751603</v>
-          </cell>
-          <cell r="C8">
-            <v>0.68375306806317004</v>
+            <v>0.93341003636238695</v>
           </cell>
         </row>
         <row r="9">
           <cell r="B9">
-            <v>0.55020390702129496</v>
-          </cell>
-          <cell r="C9">
-            <v>0.56879996507091501</v>
+            <v>0.90285564868886103</v>
           </cell>
         </row>
         <row r="10">
           <cell r="B10">
-            <v>0.67676143724751603</v>
-          </cell>
-          <cell r="C10">
-            <v>0.68375306806317004</v>
+            <v>0.93341003636238695</v>
           </cell>
         </row>
       </sheetData>
@@ -1196,7 +1342,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="7" t="str">
@@ -1225,7 +1371,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="10"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="7" t="str">
         <f>[1]tfidf_results!A3</f>
         <v>fear</v>
@@ -1252,7 +1398,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="10"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="7" t="str">
         <f>[1]tfidf_results!A4</f>
         <v>joy</v>
@@ -1279,7 +1425,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="10"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="7" t="str">
         <f>[1]tfidf_results!A5</f>
         <v>love</v>
@@ -1306,7 +1452,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="7" t="str">
         <f>[1]tfidf_results!A6</f>
         <v>sadness</v>
@@ -1333,7 +1479,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="7" t="str">
         <f>[1]tfidf_results!A7</f>
         <v>surprise</v>
@@ -1360,7 +1506,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="10"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1369,7 +1515,7 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="10"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
@@ -1395,7 +1541,7 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="10"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
@@ -1421,19 +1567,19 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="2:8" ht="17" x14ac:dyDescent="0.4">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="9">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B10)</f>
         <v>0.858512962955012</v>
@@ -1496,11 +1642,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543AA1EA-9BC7-4F6A-918E-A30F4C4A2D04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84824639-AA8B-4B07-B2C7-EE70BC8CA11C}">
   <dimension ref="B4:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1511,21 +1657,22 @@
     <col min="4" max="8" width="12.26953125" style="2" customWidth="1"/>
     <col min="9" max="9" width="1.453125" style="2" customWidth="1"/>
     <col min="10" max="11" width="12.26953125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="2"/>
+    <col min="12" max="12" width="1.6328125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" s="24" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D4" s="23" t="s">
+    <row r="4" spans="2:11" s="16" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="J4" s="23" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="J4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="22"/>
+      <c r="K4" s="23"/>
     </row>
     <row r="5" spans="2:11" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
@@ -1553,7 +1700,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="7" t="str">
@@ -1581,16 +1728,16 @@
         <v>0.82973139857980804</v>
       </c>
       <c r="J6" s="8">
-        <f>[3]w2v_results!C2</f>
+        <f>[2]w2v_results!C2</f>
         <v>0.56323465817509899</v>
       </c>
       <c r="K6" s="8">
-        <f>[3]w2v_results!B2</f>
+        <f>[2]w2v_results!B2</f>
         <v>0.58701890946259305</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="10"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="7" t="str">
         <f>[1]tfidf_results!A3</f>
         <v>fear</v>
@@ -1616,16 +1763,16 @@
         <v>0.82915194989622398</v>
       </c>
       <c r="J7" s="8">
-        <f>[3]w2v_results!C3</f>
+        <f>[2]w2v_results!C3</f>
         <v>0.54900778931750704</v>
       </c>
       <c r="K7" s="8">
-        <f>[3]w2v_results!B3</f>
+        <f>[2]w2v_results!B3</f>
         <v>0.56055267062314496</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="10"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="7" t="str">
         <f>[1]tfidf_results!A4</f>
         <v>joy</v>
@@ -1651,16 +1798,16 @@
         <v>0.93053890688362295</v>
       </c>
       <c r="J8" s="8">
-        <f>[3]w2v_results!C4</f>
+        <f>[2]w2v_results!C4</f>
         <v>0.83239425184703997</v>
       </c>
       <c r="K8" s="8">
-        <f>[3]w2v_results!B4</f>
+        <f>[2]w2v_results!B4</f>
         <v>0.84596898595437198</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="10"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="7" t="str">
         <f>[1]tfidf_results!A5</f>
         <v>love</v>
@@ -1686,16 +1833,16 @@
         <v>0.66312131423757303</v>
       </c>
       <c r="J9" s="8">
-        <f>[3]w2v_results!C5</f>
+        <f>[2]w2v_results!C5</f>
         <v>0.33467417538214</v>
       </c>
       <c r="K9" s="8">
-        <f>[3]w2v_results!B5</f>
+        <f>[2]w2v_results!B5</f>
         <v>0.22257978010190399</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="7" t="str">
         <f>[1]tfidf_results!A6</f>
         <v>sadness</v>
@@ -1721,16 +1868,16 @@
         <v>0.89903168883550499</v>
       </c>
       <c r="J10" s="8">
-        <f>[3]w2v_results!C6</f>
+        <f>[2]w2v_results!C6</f>
         <v>0.75984214799569405</v>
       </c>
       <c r="K10" s="8">
-        <f>[3]w2v_results!B6</f>
+        <f>[2]w2v_results!B6</f>
         <v>0.73867562923660801</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="7" t="str">
         <f>[1]tfidf_results!A7</f>
         <v>surprise</v>
@@ -1756,16 +1903,16 @@
         <v>0.62310214988460999</v>
       </c>
       <c r="J11" s="8">
-        <f>[3]w2v_results!C7</f>
+        <f>[2]w2v_results!C7</f>
         <v>0.37364676770801097</v>
       </c>
       <c r="K11" s="8">
-        <f>[3]w2v_results!B7</f>
+        <f>[2]w2v_results!B7</f>
         <v>0.34642746674914898</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="10"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1776,7 +1923,7 @@
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B13" s="10"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
@@ -1801,16 +1948,16 @@
         <v>0.86277599137949501</v>
       </c>
       <c r="J13" s="8">
-        <f>[3]w2v_results!C8</f>
+        <f>[2]w2v_results!C8</f>
         <v>0.68375306806317004</v>
       </c>
       <c r="K13" s="8">
-        <f>[3]w2v_results!B8</f>
+        <f>[2]w2v_results!B8</f>
         <v>0.67676143724751603</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="10"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
@@ -1835,28 +1982,28 @@
         <v>0.79577956805289096</v>
       </c>
       <c r="J14" s="8">
-        <f>[3]w2v_results!C9</f>
+        <f>[2]w2v_results!C9</f>
         <v>0.56879996507091501</v>
       </c>
       <c r="K14" s="8">
-        <f>[3]w2v_results!B9</f>
+        <f>[2]w2v_results!B9</f>
         <v>0.55020390702129496</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="2:11" ht="17" x14ac:dyDescent="0.4">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="9">
         <f>_xlfn.NUMBERVALUE([1]tfidf_results!B10)</f>
         <v>0.858512962955012</v>
@@ -1878,11 +2025,11 @@
         <v>0.86277599137949501</v>
       </c>
       <c r="J16" s="9">
-        <f>[3]w2v_results!C10</f>
+        <f>[2]w2v_results!C10</f>
         <v>0.68375306806317004</v>
       </c>
       <c r="K16" s="9">
-        <f>[3]w2v_results!B10</f>
+        <f>[2]w2v_results!B10</f>
         <v>0.67676143724751603</v>
       </c>
     </row>
@@ -1897,14 +2044,14 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="B6:B14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:K14">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="D6:L14">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0.6"/>
@@ -1915,8 +2062,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:K16">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="D16:L16">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0.84"/>
         <cfvo type="max"/>
@@ -1930,218 +2077,699 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543AA1EA-9BC7-4F6A-918E-A30F4C4A2D04}">
+  <dimension ref="B4:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="5.08984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="4" customWidth="1"/>
+    <col min="4" max="8" width="12.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="1.453125" style="2" customWidth="1"/>
+    <col min="10" max="11" width="12.26953125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="1.6328125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="14.08984375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:13" s="16" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D4" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="J4" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="23"/>
+      <c r="M4" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f>[1]tfidf_results!A2</f>
+        <v>anger</v>
+      </c>
+      <c r="D6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B2)</f>
+        <v>0.79885767212102499</v>
+      </c>
+      <c r="E6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C2)</f>
+        <v>0.84902747761654795</v>
+      </c>
+      <c r="F6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D2)</f>
+        <v>0.82630441494288298</v>
+      </c>
+      <c r="G6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E2)</f>
+        <v>0.81404754553874603</v>
+      </c>
+      <c r="H6" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F2)</f>
+        <v>0.82973139857980804</v>
+      </c>
+      <c r="J6" s="8">
+        <f>[2]w2v_results!C2</f>
+        <v>0.56323465817509899</v>
+      </c>
+      <c r="K6" s="8">
+        <f>[2]w2v_results!B2</f>
+        <v>0.58701890946259305</v>
+      </c>
+      <c r="M6" s="8">
+        <f>[4]bert_results!B2</f>
+        <v>0.90571163939487498</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B7" s="17"/>
+      <c r="C7" s="7" t="str">
+        <f>[1]tfidf_results!A3</f>
+        <v>fear</v>
+      </c>
+      <c r="D7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B3)</f>
+        <v>0.75090121254050901</v>
+      </c>
+      <c r="E7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C3)</f>
+        <v>0.80675818373812003</v>
+      </c>
+      <c r="F7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D3)</f>
+        <v>0.82321669154862898</v>
+      </c>
+      <c r="G7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E3)</f>
+        <v>0.83406765466263699</v>
+      </c>
+      <c r="H7" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F3)</f>
+        <v>0.82915194989622398</v>
+      </c>
+      <c r="J7" s="8">
+        <f>[2]w2v_results!C3</f>
+        <v>0.54900778931750704</v>
+      </c>
+      <c r="K7" s="8">
+        <f>[2]w2v_results!B3</f>
+        <v>0.56055267062314496</v>
+      </c>
+      <c r="M7" s="8">
+        <f>[4]bert_results!B3</f>
+        <v>0.89946473436987895</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B8" s="17"/>
+      <c r="C8" s="7" t="str">
+        <f>[1]tfidf_results!A4</f>
+        <v>joy</v>
+      </c>
+      <c r="D8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B4)</f>
+        <v>0.96708663827182495</v>
+      </c>
+      <c r="E8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C4)</f>
+        <v>0.94125073325001896</v>
+      </c>
+      <c r="F8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D4)</f>
+        <v>0.96002193373970202</v>
+      </c>
+      <c r="G8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E4)</f>
+        <v>0.92098752837358699</v>
+      </c>
+      <c r="H8" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F4)</f>
+        <v>0.93053890688362295</v>
+      </c>
+      <c r="J8" s="8">
+        <f>[2]w2v_results!C4</f>
+        <v>0.83239425184703997</v>
+      </c>
+      <c r="K8" s="8">
+        <f>[2]w2v_results!B4</f>
+        <v>0.84596898595437198</v>
+      </c>
+      <c r="M8" s="8">
+        <f>[4]bert_results!B4</f>
+        <v>0.93714453314290003</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B9" s="17"/>
+      <c r="C9" s="7" t="str">
+        <f>[1]tfidf_results!A5</f>
+        <v>love</v>
+      </c>
+      <c r="D9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B5)</f>
+        <v>0.555497051390059</v>
+      </c>
+      <c r="E9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C5)</f>
+        <v>0.75842459983150801</v>
+      </c>
+      <c r="F9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D5)</f>
+        <v>0.69002737994945196</v>
+      </c>
+      <c r="G9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E5)</f>
+        <v>0.67965459140690798</v>
+      </c>
+      <c r="H9" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F5)</f>
+        <v>0.66312131423757303</v>
+      </c>
+      <c r="J9" s="8">
+        <f>[2]w2v_results!C5</f>
+        <v>0.33467417538214</v>
+      </c>
+      <c r="K9" s="8">
+        <f>[2]w2v_results!B5</f>
+        <v>0.22257978010190399</v>
+      </c>
+      <c r="M9" s="8">
+        <f>[4]bert_results!B5</f>
+        <v>0.87937026116259398</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B10" s="17"/>
+      <c r="C10" s="7" t="str">
+        <f>[1]tfidf_results!A6</f>
+        <v>sadness</v>
+      </c>
+      <c r="D10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B6)</f>
+        <v>0.94311727983154603</v>
+      </c>
+      <c r="E10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C6)</f>
+        <v>0.92805136646054798</v>
+      </c>
+      <c r="F10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D6)</f>
+        <v>0.92659815828106196</v>
+      </c>
+      <c r="G10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E6)</f>
+        <v>0.88623455966309295</v>
+      </c>
+      <c r="H10" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F6)</f>
+        <v>0.89903168883550499</v>
+      </c>
+      <c r="J10" s="8">
+        <f>[2]w2v_results!C6</f>
+        <v>0.75984214799569405</v>
+      </c>
+      <c r="K10" s="8">
+        <f>[2]w2v_results!B6</f>
+        <v>0.73867562923660801</v>
+      </c>
+      <c r="M10" s="8">
+        <f>[4]bert_results!B6</f>
+        <v>0.98662455328677101</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B11" s="17"/>
+      <c r="C11" s="7" t="str">
+        <f>[1]tfidf_results!A7</f>
+        <v>surprise</v>
+      </c>
+      <c r="D11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B7)</f>
+        <v>0.42402526418073599</v>
+      </c>
+      <c r="E11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C7)</f>
+        <v>0.72585934653224804</v>
+      </c>
+      <c r="F11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D7)</f>
+        <v>0.65504676302684295</v>
+      </c>
+      <c r="G11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E7)</f>
+        <v>0.61994412729260295</v>
+      </c>
+      <c r="H11" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F7)</f>
+        <v>0.62310214988460999</v>
+      </c>
+      <c r="J11" s="8">
+        <f>[2]w2v_results!C7</f>
+        <v>0.37364676770801097</v>
+      </c>
+      <c r="K11" s="8">
+        <f>[2]w2v_results!B7</f>
+        <v>0.34642746674914898</v>
+      </c>
+      <c r="M11" s="8">
+        <f>[4]bert_results!B7</f>
+        <v>0.80881817077614404</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="17"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="17"/>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B8)</f>
+        <v>0.858512962955012</v>
+      </c>
+      <c r="E13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C8)</f>
+        <v>0.88622908733412598</v>
+      </c>
+      <c r="F13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D8)</f>
+        <v>0.88282896798650201</v>
+      </c>
+      <c r="G13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E8)</f>
+        <v>0.85549063464601405</v>
+      </c>
+      <c r="H13" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F8)</f>
+        <v>0.86277599137949501</v>
+      </c>
+      <c r="J13" s="8">
+        <f>[2]w2v_results!C8</f>
+        <v>0.68375306806317004</v>
+      </c>
+      <c r="K13" s="8">
+        <f>[2]w2v_results!B8</f>
+        <v>0.67676143724751603</v>
+      </c>
+      <c r="M13" s="8">
+        <f>[4]bert_results!B8</f>
+        <v>0.93341003636238695</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="17"/>
+      <c r="C14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B9)</f>
+        <v>0.73991418638928297</v>
+      </c>
+      <c r="E14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C9)</f>
+        <v>0.83489528457149798</v>
+      </c>
+      <c r="F14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D9)</f>
+        <v>0.81353589024809503</v>
+      </c>
+      <c r="G14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E9)</f>
+        <v>0.79248933448959502</v>
+      </c>
+      <c r="H14" s="8">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F9)</f>
+        <v>0.79577956805289096</v>
+      </c>
+      <c r="J14" s="8">
+        <f>[2]w2v_results!C9</f>
+        <v>0.56879996507091501</v>
+      </c>
+      <c r="K14" s="8">
+        <f>[2]w2v_results!B9</f>
+        <v>0.55020390702129496</v>
+      </c>
+      <c r="M14" s="8">
+        <f>[4]bert_results!B9</f>
+        <v>0.90285564868886103</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="2:13" ht="17" x14ac:dyDescent="0.4">
+      <c r="B16" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!B10)</f>
+        <v>0.858512962955012</v>
+      </c>
+      <c r="E16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!C10)</f>
+        <v>0.88622908733412598</v>
+      </c>
+      <c r="F16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!D10)</f>
+        <v>0.88282896798650201</v>
+      </c>
+      <c r="G16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!E10)</f>
+        <v>0.85549063464601405</v>
+      </c>
+      <c r="H16" s="9">
+        <f>_xlfn.NUMBERVALUE([1]tfidf_results!F10)</f>
+        <v>0.86277599137949501</v>
+      </c>
+      <c r="J16" s="9">
+        <f>[2]w2v_results!C10</f>
+        <v>0.68375306806317004</v>
+      </c>
+      <c r="K16" s="9">
+        <f>[2]w2v_results!B10</f>
+        <v>0.67676143724751603</v>
+      </c>
+      <c r="M16" s="9">
+        <f>[4]bert_results!B10</f>
+        <v>0.93341003636238695</v>
+      </c>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="J4:K4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6:M14">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:M16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0.84"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66472120-7198-4781-AF1D-D899A06886A7}">
   <dimension ref="E7:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="8.7265625" style="2"/>
     <col min="5" max="5" width="15.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="10" customWidth="1"/>
     <col min="7" max="7" width="15.81640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" style="10" customWidth="1"/>
     <col min="9" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="7" spans="5:8" ht="16.5" x14ac:dyDescent="0.4">
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E9" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!B2</f>
+      <c r="E9" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!B2</f>
         <v>compassionate</v>
       </c>
-      <c r="F9" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C2)</f>
+      <c r="F9" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C2)</f>
         <v>0.95496189594268799</v>
       </c>
-      <c r="G9" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D2</f>
+      <c r="G9" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D2</f>
         <v>playful</v>
       </c>
-      <c r="H9" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E2)</f>
+      <c r="H9" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E2)</f>
         <v>0.65957385301589899</v>
       </c>
     </row>
     <row r="10" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E10" s="20" t="str">
-        <f>[2]w2v_simlarity_affectionate!B3</f>
+      <c r="E10" s="13" t="str">
+        <f>[3]w2v_simlarity_affectionate!B3</f>
         <v>hateful</v>
       </c>
-      <c r="F10" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C3)</f>
+      <c r="F10" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C3)</f>
         <v>0.95203375816345204</v>
       </c>
-      <c r="G10" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D3</f>
+      <c r="G10" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D3</f>
         <v>loving</v>
       </c>
-      <c r="H10" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E3)</f>
+      <c r="H10" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E3)</f>
         <v>0.60796582698821999</v>
       </c>
     </row>
     <row r="11" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E11" s="20" t="str">
-        <f>[2]w2v_simlarity_affectionate!B4</f>
+      <c r="E11" s="13" t="str">
+        <f>[3]w2v_simlarity_affectionate!B4</f>
         <v>submissive</v>
       </c>
-      <c r="F11" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C4)</f>
+      <c r="F11" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C4)</f>
         <v>0.94677948951721103</v>
       </c>
-      <c r="G11" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D4</f>
+      <c r="G11" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D4</f>
         <v>endearing</v>
       </c>
-      <c r="H11" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E4)</f>
+      <c r="H11" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E4)</f>
         <v>0.605651974678039</v>
       </c>
     </row>
     <row r="12" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E12" s="21" t="str">
-        <f>[2]w2v_simlarity_affectionate!B5</f>
+      <c r="E12" s="14" t="str">
+        <f>[3]w2v_simlarity_affectionate!B5</f>
         <v>considerate</v>
       </c>
-      <c r="F12" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C5)</f>
+      <c r="F12" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C5)</f>
         <v>0.94416922330856301</v>
       </c>
-      <c r="G12" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D5</f>
+      <c r="G12" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D5</f>
         <v>affection</v>
       </c>
-      <c r="H12" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E5)</f>
+      <c r="H12" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E5)</f>
         <v>0.57452005147933904</v>
       </c>
     </row>
     <row r="13" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E13" s="20" t="str">
-        <f>[2]w2v_simlarity_affectionate!B6</f>
+      <c r="E13" s="13" t="str">
+        <f>[3]w2v_simlarity_affectionate!B6</f>
         <v>hostile</v>
       </c>
-      <c r="F13" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C6)</f>
+      <c r="F13" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C6)</f>
         <v>0.94069105386733998</v>
       </c>
-      <c r="G13" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D6</f>
+      <c r="G13" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D6</f>
         <v>flirtatious</v>
       </c>
-      <c r="H13" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E6)</f>
+      <c r="H13" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E6)</f>
         <v>0.55764240026473999</v>
       </c>
     </row>
     <row r="14" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E14" s="20" t="str">
-        <f>[2]w2v_simlarity_affectionate!B7</f>
+      <c r="E14" s="13" t="str">
+        <f>[3]w2v_simlarity_affectionate!B7</f>
         <v>unfriendly</v>
       </c>
-      <c r="F14" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C7)</f>
+      <c r="F14" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C7)</f>
         <v>0.93680131435394198</v>
       </c>
-      <c r="G14" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D7</f>
+      <c r="G14" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D7</f>
         <v>lovable</v>
       </c>
-      <c r="H14" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E7)</f>
+      <c r="H14" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E7)</f>
         <v>0.54936665296554499</v>
       </c>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E15" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!B8</f>
+      <c r="E15" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!B8</f>
         <v>truthful</v>
       </c>
-      <c r="F15" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C8)</f>
+      <c r="F15" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C8)</f>
         <v>0.93627226352691595</v>
       </c>
-      <c r="G15" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D8</f>
+      <c r="G15" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D8</f>
         <v>gentle</v>
       </c>
-      <c r="H15" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E8)</f>
+      <c r="H15" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E8)</f>
         <v>0.54669177532196001</v>
       </c>
     </row>
     <row r="16" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E16" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!B9</f>
+      <c r="E16" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!B9</f>
         <v>sympathetic</v>
       </c>
-      <c r="F16" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C9)</f>
+      <c r="F16" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C9)</f>
         <v>0.93433755636215199</v>
       </c>
-      <c r="G16" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D9</f>
+      <c r="G16" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D9</f>
         <v>sociable</v>
       </c>
-      <c r="H16" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E9)</f>
+      <c r="H16" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E9)</f>
         <v>0.5462646484375</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E17" s="20" t="str">
-        <f>[2]w2v_simlarity_affectionate!B10</f>
+      <c r="E17" s="13" t="str">
+        <f>[3]w2v_simlarity_affectionate!B10</f>
         <v>insincere</v>
       </c>
-      <c r="F17" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C10)</f>
+      <c r="F17" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C10)</f>
         <v>0.929573655128479</v>
       </c>
-      <c r="G17" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D10</f>
+      <c r="G17" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D10</f>
         <v>good_natured</v>
       </c>
-      <c r="H17" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E10)</f>
+      <c r="H17" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E10)</f>
         <v>0.54552960395812899</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E18" s="20" t="str">
-        <f>[2]w2v_simlarity_affectionate!B11</f>
+      <c r="E18" s="13" t="str">
+        <f>[3]w2v_simlarity_affectionate!B11</f>
         <v>victimized</v>
       </c>
-      <c r="F18" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!C11)</f>
+      <c r="F18" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C11)</f>
         <v>0.92484968900680498</v>
       </c>
-      <c r="G18" s="18" t="str">
-        <f>[2]w2v_simlarity_affectionate!D11</f>
+      <c r="G18" s="11" t="str">
+        <f>[3]w2v_simlarity_affectionate!D11</f>
         <v>charming</v>
       </c>
-      <c r="H18" s="19">
-        <f>_xlfn.NUMBERVALUE([2]w2v_simlarity_affectionate!E11)</f>
+      <c r="H18" s="12">
+        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E11)</f>
         <v>0.52578264474868697</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove hierarchical classification section. Add details GPT generated samples
</commit_message>
<xml_diff>
--- a/results/Display Results.xlsx
+++ b/results/Display Results.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garim\Downloads\Portfolio_ML\emotional_classification\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6224E6AD-110B-4209-9851-A8133DB9CEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1320AF19-5D59-435B-B8C2-415ED951C712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" activeTab="2" xr2:uid="{71182A3D-F6EC-4B17-9398-B1568EC59A44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" firstSheet="1" activeTab="4" xr2:uid="{71182A3D-F6EC-4B17-9398-B1568EC59A44}"/>
   </bookViews>
   <sheets>
     <sheet name="TFIDF Compare" sheetId="1" r:id="rId1"/>
     <sheet name="TFIDF W2V Compare" sheetId="5" r:id="rId2"/>
     <sheet name="TFIDF W2V BERT Compare" sheetId="3" r:id="rId3"/>
     <sheet name="Google vs Custom W2V Similarity" sheetId="2" r:id="rId4"/>
+    <sheet name="GPT Samples" sheetId="6" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Multinomial
 Naïve Bayes</t>
@@ -104,12 +106,42 @@
   <si>
     <t>Neural Network Classifier</t>
   </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>anger</t>
+  </si>
+  <si>
+    <t>fear</t>
+  </si>
+  <si>
+    <t>joy</t>
+  </si>
+  <si>
+    <t>love</t>
+  </si>
+  <si>
+    <t>sadness</t>
+  </si>
+  <si>
+    <t>surprise</t>
+  </si>
+  <si>
+    <t>Predicted Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +204,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,13 +370,61 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF98DC80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF98DC80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF98DC80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF98DC80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -778,148 +866,53 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="w2v_simlarity_affectionate"/>
+      <sheetName val="bert_results"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
-          <cell r="B2" t="str">
-            <v>compassionate</v>
-          </cell>
-          <cell r="C2">
-            <v>0.95496189594268799</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>playful</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>0.6595738530158997</v>
+          <cell r="B2">
+            <v>0.90571163939487498</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="B3" t="str">
-            <v>hateful</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>0.9520337581634521</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>loving</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v>0.6079658269882202</v>
+          <cell r="B3">
+            <v>0.89946473436987895</v>
           </cell>
         </row>
         <row r="4">
-          <cell r="B4" t="str">
-            <v>submissive</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>0.9467794895172119</v>
-          </cell>
-          <cell r="D4" t="str">
-            <v>endearing</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>0.6056519746780396</v>
+          <cell r="B4">
+            <v>0.93714453314290003</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="B5" t="str">
-            <v>considerate</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>0.9441692233085632</v>
-          </cell>
-          <cell r="D5" t="str">
-            <v>affection</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>0.5745200514793396</v>
+          <cell r="B5">
+            <v>0.87937026116259398</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="B6" t="str">
-            <v>hostile</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>0.9406910538673401</v>
-          </cell>
-          <cell r="D6" t="str">
-            <v>flirtatious</v>
-          </cell>
-          <cell r="E6">
-            <v>0.55764240026473999</v>
+          <cell r="B6">
+            <v>0.98662455328677101</v>
           </cell>
         </row>
         <row r="7">
-          <cell r="B7" t="str">
-            <v>unfriendly</v>
-          </cell>
-          <cell r="C7" t="str">
-            <v>0.9368013143539429</v>
-          </cell>
-          <cell r="D7" t="str">
-            <v>lovable</v>
-          </cell>
-          <cell r="E7" t="str">
-            <v>0.5493666529655457</v>
+          <cell r="B7">
+            <v>0.80881817077614404</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="B8" t="str">
-            <v>truthful</v>
-          </cell>
-          <cell r="C8" t="str">
-            <v>0.9362722635269165</v>
-          </cell>
-          <cell r="D8" t="str">
-            <v>gentle</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>0.5466917753219604</v>
+          <cell r="B8">
+            <v>0.93341003636238695</v>
           </cell>
         </row>
         <row r="9">
-          <cell r="B9" t="str">
-            <v>sympathetic</v>
-          </cell>
-          <cell r="C9" t="str">
-            <v>0.9343375563621521</v>
-          </cell>
-          <cell r="D9" t="str">
-            <v>sociable</v>
-          </cell>
-          <cell r="E9">
-            <v>0.5462646484375</v>
+          <cell r="B9">
+            <v>0.90285564868886103</v>
           </cell>
         </row>
         <row r="10">
-          <cell r="B10" t="str">
-            <v>insincere</v>
-          </cell>
-          <cell r="C10">
-            <v>0.929573655128479</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>good_natured</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>0.5455296039581299</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>victimized</v>
-          </cell>
-          <cell r="C11" t="str">
-            <v>0.9248496890068054</v>
-          </cell>
-          <cell r="D11" t="str">
-            <v>charming</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>0.5257826447486877</v>
+          <cell r="B10">
+            <v>0.93341003636238695</v>
           </cell>
         </row>
       </sheetData>
@@ -935,53 +928,745 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="bert_results"/>
+      <sheetName val="w2v_simlarity_affectionate"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
-          <cell r="B2">
-            <v>0.90571163939487498</v>
+          <cell r="B2" t="str">
+            <v>compassionate</v>
+          </cell>
+          <cell r="C2">
+            <v>0.95496189594268799</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>playful</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>0.6595738530158997</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="B3">
-            <v>0.89946473436987895</v>
+          <cell r="B3" t="str">
+            <v>hateful</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>0.9520337581634521</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>loving</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>0.6079658269882202</v>
           </cell>
         </row>
         <row r="4">
-          <cell r="B4">
-            <v>0.93714453314290003</v>
+          <cell r="B4" t="str">
+            <v>submissive</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>0.9467794895172119</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>endearing</v>
+          </cell>
+          <cell r="E4" t="str">
+            <v>0.6056519746780396</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="B5">
-            <v>0.87937026116259398</v>
+          <cell r="B5" t="str">
+            <v>considerate</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>0.9441692233085632</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>affection</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>0.5745200514793396</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="B6">
-            <v>0.98662455328677101</v>
+          <cell r="B6" t="str">
+            <v>hostile</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>0.9406910538673401</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>flirtatious</v>
+          </cell>
+          <cell r="E6">
+            <v>0.55764240026473999</v>
           </cell>
         </row>
         <row r="7">
-          <cell r="B7">
-            <v>0.80881817077614404</v>
+          <cell r="B7" t="str">
+            <v>unfriendly</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>0.9368013143539429</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>lovable</v>
+          </cell>
+          <cell r="E7" t="str">
+            <v>0.5493666529655457</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="B8">
-            <v>0.93341003636238695</v>
+          <cell r="B8" t="str">
+            <v>truthful</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>0.9362722635269165</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>gentle</v>
+          </cell>
+          <cell r="E8" t="str">
+            <v>0.5466917753219604</v>
           </cell>
         </row>
         <row r="9">
-          <cell r="B9">
-            <v>0.90285564868886103</v>
+          <cell r="B9" t="str">
+            <v>sympathetic</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>0.9343375563621521</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>sociable</v>
+          </cell>
+          <cell r="E9">
+            <v>0.5462646484375</v>
           </cell>
         </row>
         <row r="10">
-          <cell r="B10">
-            <v>0.93341003636238695</v>
+          <cell r="B10" t="str">
+            <v>insincere</v>
+          </cell>
+          <cell r="C10">
+            <v>0.929573655128479</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>good_natured</v>
+          </cell>
+          <cell r="E10" t="str">
+            <v>0.5455296039581299</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>victimized</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>0.9248496890068054</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>charming</v>
+          </cell>
+          <cell r="E11" t="str">
+            <v>0.5257826447486877</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="gpt_results"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>I can't believe you forgot my birthday again; this is unacceptable!</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>anger</v>
+          </cell>
+          <cell r="C2">
+            <v>0.29279013999999998</v>
+          </cell>
+          <cell r="D2">
+            <v>0.36529109999999998</v>
+          </cell>
+          <cell r="E2">
+            <v>2.7548001999999999E-2</v>
+          </cell>
+          <cell r="F2">
+            <v>2.6433540000000001E-4</v>
+          </cell>
+          <cell r="G2">
+            <v>0.31060146999999999</v>
+          </cell>
+          <cell r="H2">
+            <v>3.5049603000000002E-3</v>
+          </cell>
+          <cell r="I2" t="str">
+            <v>fear</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>I heard a noise in the dark and couldnâ€™t stop my heart from racing.</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>fear</v>
+          </cell>
+          <cell r="C3">
+            <v>2.6555615000000001E-4</v>
+          </cell>
+          <cell r="D3">
+            <v>0.99677247000000002</v>
+          </cell>
+          <cell r="E3">
+            <v>2.2407971999999999E-4</v>
+          </cell>
+          <cell r="F3">
+            <v>6.9037036000000002E-5</v>
+          </cell>
+          <cell r="G3">
+            <v>7.0257206000000003E-4</v>
+          </cell>
+          <cell r="H3">
+            <v>1.9662239999999999E-3</v>
+          </cell>
+          <cell r="I3" t="str">
+            <v>fear</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Winning the championship was the happiest moment of my life!</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>joy</v>
+          </cell>
+          <cell r="C4">
+            <v>5.6996716E-5</v>
+          </cell>
+          <cell r="D4">
+            <v>1.5359019E-3</v>
+          </cell>
+          <cell r="E4">
+            <v>0.99595814999999999</v>
+          </cell>
+          <cell r="F4">
+            <v>1.272542E-4</v>
+          </cell>
+          <cell r="G4">
+            <v>1.4808198E-3</v>
+          </cell>
+          <cell r="H4">
+            <v>8.4091090000000003E-4</v>
+          </cell>
+          <cell r="I4" t="str">
+            <v>joy</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Every moment spent with you feels like a beautiful dream come true.</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>love</v>
+          </cell>
+          <cell r="C5">
+            <v>8.3669020000000003E-5</v>
+          </cell>
+          <cell r="D5">
+            <v>2.0297208999999999E-4</v>
+          </cell>
+          <cell r="E5">
+            <v>0.98217255000000003</v>
+          </cell>
+          <cell r="F5">
+            <v>1.4258464E-2</v>
+          </cell>
+          <cell r="G5">
+            <v>5.5916473999999999E-4</v>
+          </cell>
+          <cell r="H5">
+            <v>2.7231147999999998E-3</v>
+          </cell>
+          <cell r="I5" t="str">
+            <v>joy</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>She felt an overwhelming sadness when she realized her old friend had moved away.</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>sadness</v>
+          </cell>
+          <cell r="C6">
+            <v>6.1668409999999997E-4</v>
+          </cell>
+          <cell r="D6">
+            <v>6.9568049999999999E-3</v>
+          </cell>
+          <cell r="E6">
+            <v>1.7540468E-2</v>
+          </cell>
+          <cell r="F6">
+            <v>6.1116236999999999E-3</v>
+          </cell>
+          <cell r="G6">
+            <v>0.96546200000000004</v>
+          </cell>
+          <cell r="H6">
+            <v>3.3123419000000002E-3</v>
+          </cell>
+          <cell r="I6" t="str">
+            <v>sadness</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>I was completely taken aback when I walked into the party and saw everyone there!</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>surprise</v>
+          </cell>
+          <cell r="C7">
+            <v>4.6473319999999997E-3</v>
+          </cell>
+          <cell r="D7">
+            <v>0.49863434000000001</v>
+          </cell>
+          <cell r="E7">
+            <v>1.8640397E-2</v>
+          </cell>
+          <cell r="F7">
+            <v>7.3274196000000004E-4</v>
+          </cell>
+          <cell r="G7">
+            <v>5.7719112000000003E-3</v>
+          </cell>
+          <cell r="H7">
+            <v>0.47157325999999999</v>
+          </cell>
+          <cell r="I7" t="str">
+            <v>fear</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>He slammed the door in frustration after the meeting went horribly wrong.</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>anger</v>
+          </cell>
+          <cell r="C8">
+            <v>0.98777484999999998</v>
+          </cell>
+          <cell r="D8">
+            <v>5.2172327000000003E-3</v>
+          </cell>
+          <cell r="E8">
+            <v>5.0689960000000001E-5</v>
+          </cell>
+          <cell r="F8">
+            <v>1.3537905999999999E-5</v>
+          </cell>
+          <cell r="G8">
+            <v>6.9256537000000002E-3</v>
+          </cell>
+          <cell r="H8">
+            <v>1.7965767E-5</v>
+          </cell>
+          <cell r="I8" t="str">
+            <v>anger</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>The thought of speaking in public made her stomach churn with anxiety.</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>fear</v>
+          </cell>
+          <cell r="C9">
+            <v>4.8206504000000002E-3</v>
+          </cell>
+          <cell r="D9">
+            <v>0.97875440000000002</v>
+          </cell>
+          <cell r="E9">
+            <v>9.3217560000000003E-4</v>
+          </cell>
+          <cell r="F9">
+            <v>1.5474754000000001E-4</v>
+          </cell>
+          <cell r="G9">
+            <v>1.4672579E-2</v>
+          </cell>
+          <cell r="H9">
+            <v>6.6548300000000003E-4</v>
+          </cell>
+          <cell r="I9" t="str">
+            <v>fear</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Seeing the sunrise after a long night felt like a gift from the heavens.</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>joy</v>
+          </cell>
+          <cell r="C10">
+            <v>1.5131142999999999E-4</v>
+          </cell>
+          <cell r="D10">
+            <v>2.308764E-4</v>
+          </cell>
+          <cell r="E10">
+            <v>0.99320006000000005</v>
+          </cell>
+          <cell r="F10">
+            <v>5.3343150000000001E-3</v>
+          </cell>
+          <cell r="G10">
+            <v>6.5573910000000005E-4</v>
+          </cell>
+          <cell r="H10">
+            <v>4.2767670000000001E-4</v>
+          </cell>
+          <cell r="I10" t="str">
+            <v>joy</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>His sweet words and gentle touch made her fall deeper in love every day.</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>love</v>
+          </cell>
+          <cell r="C11">
+            <v>2.4182730999999999E-3</v>
+          </cell>
+          <cell r="D11">
+            <v>1.1579255E-2</v>
+          </cell>
+          <cell r="E11">
+            <v>0.45884683999999998</v>
+          </cell>
+          <cell r="F11">
+            <v>0.48847663000000002</v>
+          </cell>
+          <cell r="G11">
+            <v>3.5776198000000002E-2</v>
+          </cell>
+          <cell r="H11">
+            <v>2.9028209999999999E-3</v>
+          </cell>
+          <cell r="I11" t="str">
+            <v>love</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>I was furious when I discovered that someone had tampered with my work.</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>anger</v>
+          </cell>
+          <cell r="C12">
+            <v>0.99099123</v>
+          </cell>
+          <cell r="D12">
+            <v>5.8599053999999996E-3</v>
+          </cell>
+          <cell r="E12">
+            <v>4.6217532000000002E-4</v>
+          </cell>
+          <cell r="F12">
+            <v>8.1037689999999998E-5</v>
+          </cell>
+          <cell r="G12">
+            <v>2.4206785000000001E-3</v>
+          </cell>
+          <cell r="H12">
+            <v>1.8504786000000001E-4</v>
+          </cell>
+          <cell r="I12" t="str">
+            <v>anger</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>The eerie silence in the abandoned house made me shiver with dread.</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>fear</v>
+          </cell>
+          <cell r="C13">
+            <v>4.9011089999999998E-3</v>
+          </cell>
+          <cell r="D13">
+            <v>0.96755990000000003</v>
+          </cell>
+          <cell r="E13">
+            <v>2.1281999999999998E-3</v>
+          </cell>
+          <cell r="F13">
+            <v>4.5380596000000001E-4</v>
+          </cell>
+          <cell r="G13">
+            <v>1.0668449E-2</v>
+          </cell>
+          <cell r="H13">
+            <v>1.4288633E-2</v>
+          </cell>
+          <cell r="I13" t="str">
+            <v>fear</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>The laughter of children playing in the park filled my heart with pure joy.</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>joy</v>
+          </cell>
+          <cell r="C14">
+            <v>2.6485390000000002E-5</v>
+          </cell>
+          <cell r="D14">
+            <v>4.1904216000000002E-4</v>
+          </cell>
+          <cell r="E14">
+            <v>0.99579406000000004</v>
+          </cell>
+          <cell r="F14">
+            <v>6.6701206000000001E-4</v>
+          </cell>
+          <cell r="G14">
+            <v>3.4222175999999997E-4</v>
+          </cell>
+          <cell r="H14">
+            <v>2.7511797000000001E-3</v>
+          </cell>
+          <cell r="I14" t="str">
+            <v>joy</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>Their long walks together in the moonlight showed how deeply they cared for each other.</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>love</v>
+          </cell>
+          <cell r="C15">
+            <v>7.6481460000000004E-4</v>
+          </cell>
+          <cell r="D15">
+            <v>4.7552654999999996E-3</v>
+          </cell>
+          <cell r="E15">
+            <v>0.22035436</v>
+          </cell>
+          <cell r="F15">
+            <v>0.75720240000000005</v>
+          </cell>
+          <cell r="G15">
+            <v>1.4654439999999999E-2</v>
+          </cell>
+          <cell r="H15">
+            <v>2.2687647000000002E-3</v>
+          </cell>
+          <cell r="I15" t="str">
+            <v>love</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>He felt a deep sadness as he watched the final credits roll on the movie he had loved.</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>sadness</v>
+          </cell>
+          <cell r="C16">
+            <v>1.0048780000000001E-3</v>
+          </cell>
+          <cell r="D16">
+            <v>8.4161140000000006E-3</v>
+          </cell>
+          <cell r="E16">
+            <v>0.19092333</v>
+          </cell>
+          <cell r="F16">
+            <v>0.12880411999999999</v>
+          </cell>
+          <cell r="G16">
+            <v>0.66572209999999998</v>
+          </cell>
+          <cell r="H16">
+            <v>5.1295296000000001E-3</v>
+          </cell>
+          <cell r="I16" t="str">
+            <v>sadness</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>She was astonished to find a surprise letter from her old friend waiting on her desk.</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>surprise</v>
+          </cell>
+          <cell r="C17">
+            <v>2.0319772999999999E-2</v>
+          </cell>
+          <cell r="D17">
+            <v>0.17401077000000001</v>
+          </cell>
+          <cell r="E17">
+            <v>0.5158509</v>
+          </cell>
+          <cell r="F17">
+            <v>1.2495077E-2</v>
+          </cell>
+          <cell r="G17">
+            <v>9.7109585999999998E-2</v>
+          </cell>
+          <cell r="H17">
+            <v>0.18021390000000001</v>
+          </cell>
+          <cell r="I17" t="str">
+            <v>joy</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>The constant delays and excuses from the company made me lose my patience.</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>anger</v>
+          </cell>
+          <cell r="C18">
+            <v>0.88482830000000001</v>
+          </cell>
+          <cell r="D18">
+            <v>4.1374117000000002E-2</v>
+          </cell>
+          <cell r="E18">
+            <v>1.4967945E-3</v>
+          </cell>
+          <cell r="F18">
+            <v>2.3871103999999999E-4</v>
+          </cell>
+          <cell r="G18">
+            <v>7.1745840000000005E-2</v>
+          </cell>
+          <cell r="H18">
+            <v>3.1624426000000002E-4</v>
+          </cell>
+          <cell r="I18" t="str">
+            <v>anger</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Driving through the foggy night, he could barely see a few feet ahead, feeling a chill of fear.</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>fear</v>
+          </cell>
+          <cell r="C19">
+            <v>1.07949E-2</v>
+          </cell>
+          <cell r="D19">
+            <v>0.98475250000000003</v>
+          </cell>
+          <cell r="E19">
+            <v>4.7142978000000002E-4</v>
+          </cell>
+          <cell r="F19">
+            <v>3.5953932E-4</v>
+          </cell>
+          <cell r="G19">
+            <v>5.1585864000000005E-4</v>
+          </cell>
+          <cell r="H19">
+            <v>3.1058344000000002E-3</v>
+          </cell>
+          <cell r="I19" t="str">
+            <v>fear</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Her face lit up with joy when she saw the beautiful, unexpected gift.</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>joy</v>
+          </cell>
+          <cell r="C20">
+            <v>4.2080745999999998E-6</v>
+          </cell>
+          <cell r="D20">
+            <v>5.050541E-5</v>
+          </cell>
+          <cell r="E20">
+            <v>0.99750536999999995</v>
+          </cell>
+          <cell r="F20">
+            <v>1.4053572999999999E-4</v>
+          </cell>
+          <cell r="G20">
+            <v>3.7942960000000003E-5</v>
+          </cell>
+          <cell r="H20">
+            <v>2.2614808E-3</v>
+          </cell>
+          <cell r="I20" t="str">
+            <v>joy</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>Every day, he made sure to remind her how much he loved her with little gestures and kind words.</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>love</v>
+          </cell>
+          <cell r="C21">
+            <v>1.7888928000000001E-3</v>
+          </cell>
+          <cell r="D21">
+            <v>3.8236912999999998E-3</v>
+          </cell>
+          <cell r="E21">
+            <v>0.37963805</v>
+          </cell>
+          <cell r="F21">
+            <v>0.59053560000000005</v>
+          </cell>
+          <cell r="G21">
+            <v>2.3350513E-2</v>
+          </cell>
+          <cell r="H21">
+            <v>8.6324627000000003E-4</v>
+          </cell>
+          <cell r="I21" t="str">
+            <v>love</v>
           </cell>
         </row>
       </sheetData>
@@ -2080,7 +2765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543AA1EA-9BC7-4F6A-918E-A30F4C4A2D04}">
   <dimension ref="B4:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -2178,7 +2863,7 @@
         <v>0.58701890946259305</v>
       </c>
       <c r="M6" s="8">
-        <f>[4]bert_results!B2</f>
+        <f>[3]bert_results!B2</f>
         <v>0.90571163939487498</v>
       </c>
     </row>
@@ -2217,7 +2902,7 @@
         <v>0.56055267062314496</v>
       </c>
       <c r="M7" s="8">
-        <f>[4]bert_results!B3</f>
+        <f>[3]bert_results!B3</f>
         <v>0.89946473436987895</v>
       </c>
     </row>
@@ -2256,7 +2941,7 @@
         <v>0.84596898595437198</v>
       </c>
       <c r="M8" s="8">
-        <f>[4]bert_results!B4</f>
+        <f>[3]bert_results!B4</f>
         <v>0.93714453314290003</v>
       </c>
     </row>
@@ -2295,7 +2980,7 @@
         <v>0.22257978010190399</v>
       </c>
       <c r="M9" s="8">
-        <f>[4]bert_results!B5</f>
+        <f>[3]bert_results!B5</f>
         <v>0.87937026116259398</v>
       </c>
     </row>
@@ -2334,7 +3019,7 @@
         <v>0.73867562923660801</v>
       </c>
       <c r="M10" s="8">
-        <f>[4]bert_results!B6</f>
+        <f>[3]bert_results!B6</f>
         <v>0.98662455328677101</v>
       </c>
     </row>
@@ -2373,7 +3058,7 @@
         <v>0.34642746674914898</v>
       </c>
       <c r="M11" s="8">
-        <f>[4]bert_results!B7</f>
+        <f>[3]bert_results!B7</f>
         <v>0.80881817077614404</v>
       </c>
     </row>
@@ -2423,7 +3108,7 @@
         <v>0.67676143724751603</v>
       </c>
       <c r="M13" s="8">
-        <f>[4]bert_results!B8</f>
+        <f>[3]bert_results!B8</f>
         <v>0.93341003636238695</v>
       </c>
     </row>
@@ -2461,7 +3146,7 @@
         <v>0.55020390702129496</v>
       </c>
       <c r="M14" s="8">
-        <f>[4]bert_results!B9</f>
+        <f>[3]bert_results!B9</f>
         <v>0.90285564868886103</v>
       </c>
     </row>
@@ -2508,7 +3193,7 @@
         <v>0.67676143724751603</v>
       </c>
       <c r="M16" s="9">
-        <f>[4]bert_results!B10</f>
+        <f>[3]bert_results!B10</f>
         <v>0.93341003636238695</v>
       </c>
     </row>
@@ -2595,181 +3280,181 @@
     </row>
     <row r="9" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E9" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!B2</f>
+        <f>[4]w2v_simlarity_affectionate!B2</f>
         <v>compassionate</v>
       </c>
       <c r="F9" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C2)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C2)</f>
         <v>0.95496189594268799</v>
       </c>
       <c r="G9" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D2</f>
+        <f>[4]w2v_simlarity_affectionate!D2</f>
         <v>playful</v>
       </c>
       <c r="H9" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E2)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E2)</f>
         <v>0.65957385301589899</v>
       </c>
     </row>
     <row r="10" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E10" s="13" t="str">
-        <f>[3]w2v_simlarity_affectionate!B3</f>
+        <f>[4]w2v_simlarity_affectionate!B3</f>
         <v>hateful</v>
       </c>
       <c r="F10" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C3)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C3)</f>
         <v>0.95203375816345204</v>
       </c>
       <c r="G10" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D3</f>
+        <f>[4]w2v_simlarity_affectionate!D3</f>
         <v>loving</v>
       </c>
       <c r="H10" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E3)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E3)</f>
         <v>0.60796582698821999</v>
       </c>
     </row>
     <row r="11" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E11" s="13" t="str">
-        <f>[3]w2v_simlarity_affectionate!B4</f>
+        <f>[4]w2v_simlarity_affectionate!B4</f>
         <v>submissive</v>
       </c>
       <c r="F11" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C4)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C4)</f>
         <v>0.94677948951721103</v>
       </c>
       <c r="G11" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D4</f>
+        <f>[4]w2v_simlarity_affectionate!D4</f>
         <v>endearing</v>
       </c>
       <c r="H11" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E4)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E4)</f>
         <v>0.605651974678039</v>
       </c>
     </row>
     <row r="12" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E12" s="14" t="str">
-        <f>[3]w2v_simlarity_affectionate!B5</f>
+        <f>[4]w2v_simlarity_affectionate!B5</f>
         <v>considerate</v>
       </c>
       <c r="F12" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C5)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C5)</f>
         <v>0.94416922330856301</v>
       </c>
       <c r="G12" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D5</f>
+        <f>[4]w2v_simlarity_affectionate!D5</f>
         <v>affection</v>
       </c>
       <c r="H12" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E5)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E5)</f>
         <v>0.57452005147933904</v>
       </c>
     </row>
     <row r="13" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E13" s="13" t="str">
-        <f>[3]w2v_simlarity_affectionate!B6</f>
+        <f>[4]w2v_simlarity_affectionate!B6</f>
         <v>hostile</v>
       </c>
       <c r="F13" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C6)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C6)</f>
         <v>0.94069105386733998</v>
       </c>
       <c r="G13" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D6</f>
+        <f>[4]w2v_simlarity_affectionate!D6</f>
         <v>flirtatious</v>
       </c>
       <c r="H13" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E6)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E6)</f>
         <v>0.55764240026473999</v>
       </c>
     </row>
     <row r="14" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E14" s="13" t="str">
-        <f>[3]w2v_simlarity_affectionate!B7</f>
+        <f>[4]w2v_simlarity_affectionate!B7</f>
         <v>unfriendly</v>
       </c>
       <c r="F14" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C7)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C7)</f>
         <v>0.93680131435394198</v>
       </c>
       <c r="G14" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D7</f>
+        <f>[4]w2v_simlarity_affectionate!D7</f>
         <v>lovable</v>
       </c>
       <c r="H14" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E7)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E7)</f>
         <v>0.54936665296554499</v>
       </c>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E15" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!B8</f>
+        <f>[4]w2v_simlarity_affectionate!B8</f>
         <v>truthful</v>
       </c>
       <c r="F15" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C8)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C8)</f>
         <v>0.93627226352691595</v>
       </c>
       <c r="G15" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D8</f>
+        <f>[4]w2v_simlarity_affectionate!D8</f>
         <v>gentle</v>
       </c>
       <c r="H15" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E8)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E8)</f>
         <v>0.54669177532196001</v>
       </c>
     </row>
     <row r="16" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E16" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!B9</f>
+        <f>[4]w2v_simlarity_affectionate!B9</f>
         <v>sympathetic</v>
       </c>
       <c r="F16" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C9)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C9)</f>
         <v>0.93433755636215199</v>
       </c>
       <c r="G16" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D9</f>
+        <f>[4]w2v_simlarity_affectionate!D9</f>
         <v>sociable</v>
       </c>
       <c r="H16" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E9)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E9)</f>
         <v>0.5462646484375</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E17" s="13" t="str">
-        <f>[3]w2v_simlarity_affectionate!B10</f>
+        <f>[4]w2v_simlarity_affectionate!B10</f>
         <v>insincere</v>
       </c>
       <c r="F17" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C10)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C10)</f>
         <v>0.929573655128479</v>
       </c>
       <c r="G17" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D10</f>
+        <f>[4]w2v_simlarity_affectionate!D10</f>
         <v>good_natured</v>
       </c>
       <c r="H17" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E10)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E10)</f>
         <v>0.54552960395812899</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E18" s="13" t="str">
-        <f>[3]w2v_simlarity_affectionate!B11</f>
+        <f>[4]w2v_simlarity_affectionate!B11</f>
         <v>victimized</v>
       </c>
       <c r="F18" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!C11)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!C11)</f>
         <v>0.92484968900680498</v>
       </c>
       <c r="G18" s="11" t="str">
-        <f>[3]w2v_simlarity_affectionate!D11</f>
+        <f>[4]w2v_simlarity_affectionate!D11</f>
         <v>charming</v>
       </c>
       <c r="H18" s="12">
-        <f>_xlfn.NUMBERVALUE([3]w2v_simlarity_affectionate!E11)</f>
+        <f>_xlfn.NUMBERVALUE([4]w2v_simlarity_affectionate!E11)</f>
         <v>0.52578264474868697</v>
       </c>
     </row>
@@ -2793,4 +3478,917 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E7F6F1-DB78-4F2D-A085-007A6BD5B9DD}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="30"/>
+    <col min="3" max="3" width="77.6328125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="30" customWidth="1"/>
+    <col min="5" max="10" width="8.81640625" style="30" customWidth="1"/>
+    <col min="11" max="11" width="11.1796875" style="30" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D1" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="26" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="30" t="b">
+        <f>K5=D5</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="31" t="str">
+        <f>[5]gpt_results!A2</f>
+        <v>I can't believe you forgot my birthday again; this is unacceptable!</v>
+      </c>
+      <c r="D5" s="29" t="str">
+        <f>[5]gpt_results!B2</f>
+        <v>anger</v>
+      </c>
+      <c r="E5" s="28">
+        <f>[5]gpt_results!C2</f>
+        <v>0.29279013999999998</v>
+      </c>
+      <c r="F5" s="28">
+        <f>[5]gpt_results!D2</f>
+        <v>0.36529109999999998</v>
+      </c>
+      <c r="G5" s="28">
+        <f>[5]gpt_results!E2</f>
+        <v>2.7548001999999999E-2</v>
+      </c>
+      <c r="H5" s="28">
+        <f>[5]gpt_results!F2</f>
+        <v>2.6433540000000001E-4</v>
+      </c>
+      <c r="I5" s="28">
+        <f>[5]gpt_results!G2</f>
+        <v>0.31060146999999999</v>
+      </c>
+      <c r="J5" s="28">
+        <f>[5]gpt_results!H2</f>
+        <v>3.5049603000000002E-3</v>
+      </c>
+      <c r="K5" s="29" t="str">
+        <f>[5]gpt_results!I2</f>
+        <v>fear</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="30" t="b">
+        <f t="shared" ref="A6:A24" si="0">K6=D6</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="31" t="str">
+        <f>[5]gpt_results!A3</f>
+        <v>I heard a noise in the dark and couldnâ€™t stop my heart from racing.</v>
+      </c>
+      <c r="D6" s="29" t="str">
+        <f>[5]gpt_results!B3</f>
+        <v>fear</v>
+      </c>
+      <c r="E6" s="28">
+        <f>[5]gpt_results!C3</f>
+        <v>2.6555615000000001E-4</v>
+      </c>
+      <c r="F6" s="28">
+        <f>[5]gpt_results!D3</f>
+        <v>0.99677247000000002</v>
+      </c>
+      <c r="G6" s="28">
+        <f>[5]gpt_results!E3</f>
+        <v>2.2407971999999999E-4</v>
+      </c>
+      <c r="H6" s="28">
+        <f>[5]gpt_results!F3</f>
+        <v>6.9037036000000002E-5</v>
+      </c>
+      <c r="I6" s="28">
+        <f>[5]gpt_results!G3</f>
+        <v>7.0257206000000003E-4</v>
+      </c>
+      <c r="J6" s="28">
+        <f>[5]gpt_results!H3</f>
+        <v>1.9662239999999999E-3</v>
+      </c>
+      <c r="K6" s="29" t="str">
+        <f>[5]gpt_results!I3</f>
+        <v>fear</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="31" t="str">
+        <f>[5]gpt_results!A4</f>
+        <v>Winning the championship was the happiest moment of my life!</v>
+      </c>
+      <c r="D7" s="29" t="str">
+        <f>[5]gpt_results!B4</f>
+        <v>joy</v>
+      </c>
+      <c r="E7" s="28">
+        <f>[5]gpt_results!C4</f>
+        <v>5.6996716E-5</v>
+      </c>
+      <c r="F7" s="28">
+        <f>[5]gpt_results!D4</f>
+        <v>1.5359019E-3</v>
+      </c>
+      <c r="G7" s="28">
+        <f>[5]gpt_results!E4</f>
+        <v>0.99595814999999999</v>
+      </c>
+      <c r="H7" s="28">
+        <f>[5]gpt_results!F4</f>
+        <v>1.272542E-4</v>
+      </c>
+      <c r="I7" s="28">
+        <f>[5]gpt_results!G4</f>
+        <v>1.4808198E-3</v>
+      </c>
+      <c r="J7" s="28">
+        <f>[5]gpt_results!H4</f>
+        <v>8.4091090000000003E-4</v>
+      </c>
+      <c r="K7" s="29" t="str">
+        <f>[5]gpt_results!I4</f>
+        <v>joy</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="31" t="str">
+        <f>[5]gpt_results!A5</f>
+        <v>Every moment spent with you feels like a beautiful dream come true.</v>
+      </c>
+      <c r="D8" s="29" t="str">
+        <f>[5]gpt_results!B5</f>
+        <v>love</v>
+      </c>
+      <c r="E8" s="28">
+        <f>[5]gpt_results!C5</f>
+        <v>8.3669020000000003E-5</v>
+      </c>
+      <c r="F8" s="28">
+        <f>[5]gpt_results!D5</f>
+        <v>2.0297208999999999E-4</v>
+      </c>
+      <c r="G8" s="28">
+        <f>[5]gpt_results!E5</f>
+        <v>0.98217255000000003</v>
+      </c>
+      <c r="H8" s="28">
+        <f>[5]gpt_results!F5</f>
+        <v>1.4258464E-2</v>
+      </c>
+      <c r="I8" s="28">
+        <f>[5]gpt_results!G5</f>
+        <v>5.5916473999999999E-4</v>
+      </c>
+      <c r="J8" s="28">
+        <f>[5]gpt_results!H5</f>
+        <v>2.7231147999999998E-3</v>
+      </c>
+      <c r="K8" s="29" t="str">
+        <f>[5]gpt_results!I5</f>
+        <v>joy</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C9" s="31" t="str">
+        <f>[5]gpt_results!A6</f>
+        <v>She felt an overwhelming sadness when she realized her old friend had moved away.</v>
+      </c>
+      <c r="D9" s="29" t="str">
+        <f>[5]gpt_results!B6</f>
+        <v>sadness</v>
+      </c>
+      <c r="E9" s="28">
+        <f>[5]gpt_results!C6</f>
+        <v>6.1668409999999997E-4</v>
+      </c>
+      <c r="F9" s="28">
+        <f>[5]gpt_results!D6</f>
+        <v>6.9568049999999999E-3</v>
+      </c>
+      <c r="G9" s="28">
+        <f>[5]gpt_results!E6</f>
+        <v>1.7540468E-2</v>
+      </c>
+      <c r="H9" s="28">
+        <f>[5]gpt_results!F6</f>
+        <v>6.1116236999999999E-3</v>
+      </c>
+      <c r="I9" s="28">
+        <f>[5]gpt_results!G6</f>
+        <v>0.96546200000000004</v>
+      </c>
+      <c r="J9" s="28">
+        <f>[5]gpt_results!H6</f>
+        <v>3.3123419000000002E-3</v>
+      </c>
+      <c r="K9" s="29" t="str">
+        <f>[5]gpt_results!I6</f>
+        <v>sadness</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="31" t="str">
+        <f>[5]gpt_results!A7</f>
+        <v>I was completely taken aback when I walked into the party and saw everyone there!</v>
+      </c>
+      <c r="D10" s="29" t="str">
+        <f>[5]gpt_results!B7</f>
+        <v>surprise</v>
+      </c>
+      <c r="E10" s="28">
+        <f>[5]gpt_results!C7</f>
+        <v>4.6473319999999997E-3</v>
+      </c>
+      <c r="F10" s="28">
+        <f>[5]gpt_results!D7</f>
+        <v>0.49863434000000001</v>
+      </c>
+      <c r="G10" s="28">
+        <f>[5]gpt_results!E7</f>
+        <v>1.8640397E-2</v>
+      </c>
+      <c r="H10" s="28">
+        <f>[5]gpt_results!F7</f>
+        <v>7.3274196000000004E-4</v>
+      </c>
+      <c r="I10" s="28">
+        <f>[5]gpt_results!G7</f>
+        <v>5.7719112000000003E-3</v>
+      </c>
+      <c r="J10" s="28">
+        <f>[5]gpt_results!H7</f>
+        <v>0.47157325999999999</v>
+      </c>
+      <c r="K10" s="29" t="str">
+        <f>[5]gpt_results!I7</f>
+        <v>fear</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11" s="31" t="str">
+        <f>[5]gpt_results!A8</f>
+        <v>He slammed the door in frustration after the meeting went horribly wrong.</v>
+      </c>
+      <c r="D11" s="29" t="str">
+        <f>[5]gpt_results!B8</f>
+        <v>anger</v>
+      </c>
+      <c r="E11" s="28">
+        <f>[5]gpt_results!C8</f>
+        <v>0.98777484999999998</v>
+      </c>
+      <c r="F11" s="28">
+        <f>[5]gpt_results!D8</f>
+        <v>5.2172327000000003E-3</v>
+      </c>
+      <c r="G11" s="28">
+        <f>[5]gpt_results!E8</f>
+        <v>5.0689960000000001E-5</v>
+      </c>
+      <c r="H11" s="28">
+        <f>[5]gpt_results!F8</f>
+        <v>1.3537905999999999E-5</v>
+      </c>
+      <c r="I11" s="28">
+        <f>[5]gpt_results!G8</f>
+        <v>6.9256537000000002E-3</v>
+      </c>
+      <c r="J11" s="28">
+        <f>[5]gpt_results!H8</f>
+        <v>1.7965767E-5</v>
+      </c>
+      <c r="K11" s="29" t="str">
+        <f>[5]gpt_results!I8</f>
+        <v>anger</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C12" s="31" t="str">
+        <f>[5]gpt_results!A9</f>
+        <v>The thought of speaking in public made her stomach churn with anxiety.</v>
+      </c>
+      <c r="D12" s="29" t="str">
+        <f>[5]gpt_results!B9</f>
+        <v>fear</v>
+      </c>
+      <c r="E12" s="28">
+        <f>[5]gpt_results!C9</f>
+        <v>4.8206504000000002E-3</v>
+      </c>
+      <c r="F12" s="28">
+        <f>[5]gpt_results!D9</f>
+        <v>0.97875440000000002</v>
+      </c>
+      <c r="G12" s="28">
+        <f>[5]gpt_results!E9</f>
+        <v>9.3217560000000003E-4</v>
+      </c>
+      <c r="H12" s="28">
+        <f>[5]gpt_results!F9</f>
+        <v>1.5474754000000001E-4</v>
+      </c>
+      <c r="I12" s="28">
+        <f>[5]gpt_results!G9</f>
+        <v>1.4672579E-2</v>
+      </c>
+      <c r="J12" s="28">
+        <f>[5]gpt_results!H9</f>
+        <v>6.6548300000000003E-4</v>
+      </c>
+      <c r="K12" s="29" t="str">
+        <f>[5]gpt_results!I9</f>
+        <v>fear</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C13" s="31" t="str">
+        <f>[5]gpt_results!A10</f>
+        <v>Seeing the sunrise after a long night felt like a gift from the heavens.</v>
+      </c>
+      <c r="D13" s="29" t="str">
+        <f>[5]gpt_results!B10</f>
+        <v>joy</v>
+      </c>
+      <c r="E13" s="28">
+        <f>[5]gpt_results!C10</f>
+        <v>1.5131142999999999E-4</v>
+      </c>
+      <c r="F13" s="28">
+        <f>[5]gpt_results!D10</f>
+        <v>2.308764E-4</v>
+      </c>
+      <c r="G13" s="28">
+        <f>[5]gpt_results!E10</f>
+        <v>0.99320006000000005</v>
+      </c>
+      <c r="H13" s="28">
+        <f>[5]gpt_results!F10</f>
+        <v>5.3343150000000001E-3</v>
+      </c>
+      <c r="I13" s="28">
+        <f>[5]gpt_results!G10</f>
+        <v>6.5573910000000005E-4</v>
+      </c>
+      <c r="J13" s="28">
+        <f>[5]gpt_results!H10</f>
+        <v>4.2767670000000001E-4</v>
+      </c>
+      <c r="K13" s="29" t="str">
+        <f>[5]gpt_results!I10</f>
+        <v>joy</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C14" s="31" t="str">
+        <f>[5]gpt_results!A11</f>
+        <v>His sweet words and gentle touch made her fall deeper in love every day.</v>
+      </c>
+      <c r="D14" s="29" t="str">
+        <f>[5]gpt_results!B11</f>
+        <v>love</v>
+      </c>
+      <c r="E14" s="28">
+        <f>[5]gpt_results!C11</f>
+        <v>2.4182730999999999E-3</v>
+      </c>
+      <c r="F14" s="28">
+        <f>[5]gpt_results!D11</f>
+        <v>1.1579255E-2</v>
+      </c>
+      <c r="G14" s="28">
+        <f>[5]gpt_results!E11</f>
+        <v>0.45884683999999998</v>
+      </c>
+      <c r="H14" s="28">
+        <f>[5]gpt_results!F11</f>
+        <v>0.48847663000000002</v>
+      </c>
+      <c r="I14" s="28">
+        <f>[5]gpt_results!G11</f>
+        <v>3.5776198000000002E-2</v>
+      </c>
+      <c r="J14" s="28">
+        <f>[5]gpt_results!H11</f>
+        <v>2.9028209999999999E-3</v>
+      </c>
+      <c r="K14" s="29" t="str">
+        <f>[5]gpt_results!I11</f>
+        <v>love</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C15" s="31" t="str">
+        <f>[5]gpt_results!A12</f>
+        <v>I was furious when I discovered that someone had tampered with my work.</v>
+      </c>
+      <c r="D15" s="29" t="str">
+        <f>[5]gpt_results!B12</f>
+        <v>anger</v>
+      </c>
+      <c r="E15" s="28">
+        <f>[5]gpt_results!C12</f>
+        <v>0.99099123</v>
+      </c>
+      <c r="F15" s="28">
+        <f>[5]gpt_results!D12</f>
+        <v>5.8599053999999996E-3</v>
+      </c>
+      <c r="G15" s="28">
+        <f>[5]gpt_results!E12</f>
+        <v>4.6217532000000002E-4</v>
+      </c>
+      <c r="H15" s="28">
+        <f>[5]gpt_results!F12</f>
+        <v>8.1037689999999998E-5</v>
+      </c>
+      <c r="I15" s="28">
+        <f>[5]gpt_results!G12</f>
+        <v>2.4206785000000001E-3</v>
+      </c>
+      <c r="J15" s="28">
+        <f>[5]gpt_results!H12</f>
+        <v>1.8504786000000001E-4</v>
+      </c>
+      <c r="K15" s="29" t="str">
+        <f>[5]gpt_results!I12</f>
+        <v>anger</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C16" s="31" t="str">
+        <f>[5]gpt_results!A13</f>
+        <v>The eerie silence in the abandoned house made me shiver with dread.</v>
+      </c>
+      <c r="D16" s="29" t="str">
+        <f>[5]gpt_results!B13</f>
+        <v>fear</v>
+      </c>
+      <c r="E16" s="28">
+        <f>[5]gpt_results!C13</f>
+        <v>4.9011089999999998E-3</v>
+      </c>
+      <c r="F16" s="28">
+        <f>[5]gpt_results!D13</f>
+        <v>0.96755990000000003</v>
+      </c>
+      <c r="G16" s="28">
+        <f>[5]gpt_results!E13</f>
+        <v>2.1281999999999998E-3</v>
+      </c>
+      <c r="H16" s="28">
+        <f>[5]gpt_results!F13</f>
+        <v>4.5380596000000001E-4</v>
+      </c>
+      <c r="I16" s="28">
+        <f>[5]gpt_results!G13</f>
+        <v>1.0668449E-2</v>
+      </c>
+      <c r="J16" s="28">
+        <f>[5]gpt_results!H13</f>
+        <v>1.4288633E-2</v>
+      </c>
+      <c r="K16" s="29" t="str">
+        <f>[5]gpt_results!I13</f>
+        <v>fear</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C17" s="31" t="str">
+        <f>[5]gpt_results!A14</f>
+        <v>The laughter of children playing in the park filled my heart with pure joy.</v>
+      </c>
+      <c r="D17" s="29" t="str">
+        <f>[5]gpt_results!B14</f>
+        <v>joy</v>
+      </c>
+      <c r="E17" s="28">
+        <f>[5]gpt_results!C14</f>
+        <v>2.6485390000000002E-5</v>
+      </c>
+      <c r="F17" s="28">
+        <f>[5]gpt_results!D14</f>
+        <v>4.1904216000000002E-4</v>
+      </c>
+      <c r="G17" s="28">
+        <f>[5]gpt_results!E14</f>
+        <v>0.99579406000000004</v>
+      </c>
+      <c r="H17" s="28">
+        <f>[5]gpt_results!F14</f>
+        <v>6.6701206000000001E-4</v>
+      </c>
+      <c r="I17" s="28">
+        <f>[5]gpt_results!G14</f>
+        <v>3.4222175999999997E-4</v>
+      </c>
+      <c r="J17" s="28">
+        <f>[5]gpt_results!H14</f>
+        <v>2.7511797000000001E-3</v>
+      </c>
+      <c r="K17" s="29" t="str">
+        <f>[5]gpt_results!I14</f>
+        <v>joy</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C18" s="31" t="str">
+        <f>[5]gpt_results!A15</f>
+        <v>Their long walks together in the moonlight showed how deeply they cared for each other.</v>
+      </c>
+      <c r="D18" s="29" t="str">
+        <f>[5]gpt_results!B15</f>
+        <v>love</v>
+      </c>
+      <c r="E18" s="28">
+        <f>[5]gpt_results!C15</f>
+        <v>7.6481460000000004E-4</v>
+      </c>
+      <c r="F18" s="28">
+        <f>[5]gpt_results!D15</f>
+        <v>4.7552654999999996E-3</v>
+      </c>
+      <c r="G18" s="28">
+        <f>[5]gpt_results!E15</f>
+        <v>0.22035436</v>
+      </c>
+      <c r="H18" s="28">
+        <f>[5]gpt_results!F15</f>
+        <v>0.75720240000000005</v>
+      </c>
+      <c r="I18" s="28">
+        <f>[5]gpt_results!G15</f>
+        <v>1.4654439999999999E-2</v>
+      </c>
+      <c r="J18" s="28">
+        <f>[5]gpt_results!H15</f>
+        <v>2.2687647000000002E-3</v>
+      </c>
+      <c r="K18" s="29" t="str">
+        <f>[5]gpt_results!I15</f>
+        <v>love</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C19" s="31" t="str">
+        <f>[5]gpt_results!A16</f>
+        <v>He felt a deep sadness as he watched the final credits roll on the movie he had loved.</v>
+      </c>
+      <c r="D19" s="29" t="str">
+        <f>[5]gpt_results!B16</f>
+        <v>sadness</v>
+      </c>
+      <c r="E19" s="28">
+        <f>[5]gpt_results!C16</f>
+        <v>1.0048780000000001E-3</v>
+      </c>
+      <c r="F19" s="28">
+        <f>[5]gpt_results!D16</f>
+        <v>8.4161140000000006E-3</v>
+      </c>
+      <c r="G19" s="28">
+        <f>[5]gpt_results!E16</f>
+        <v>0.19092333</v>
+      </c>
+      <c r="H19" s="28">
+        <f>[5]gpt_results!F16</f>
+        <v>0.12880411999999999</v>
+      </c>
+      <c r="I19" s="28">
+        <f>[5]gpt_results!G16</f>
+        <v>0.66572209999999998</v>
+      </c>
+      <c r="J19" s="28">
+        <f>[5]gpt_results!H16</f>
+        <v>5.1295296000000001E-3</v>
+      </c>
+      <c r="K19" s="29" t="str">
+        <f>[5]gpt_results!I16</f>
+        <v>sadness</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C20" s="31" t="str">
+        <f>[5]gpt_results!A17</f>
+        <v>She was astonished to find a surprise letter from her old friend waiting on her desk.</v>
+      </c>
+      <c r="D20" s="29" t="str">
+        <f>[5]gpt_results!B17</f>
+        <v>surprise</v>
+      </c>
+      <c r="E20" s="28">
+        <f>[5]gpt_results!C17</f>
+        <v>2.0319772999999999E-2</v>
+      </c>
+      <c r="F20" s="28">
+        <f>[5]gpt_results!D17</f>
+        <v>0.17401077000000001</v>
+      </c>
+      <c r="G20" s="28">
+        <f>[5]gpt_results!E17</f>
+        <v>0.5158509</v>
+      </c>
+      <c r="H20" s="28">
+        <f>[5]gpt_results!F17</f>
+        <v>1.2495077E-2</v>
+      </c>
+      <c r="I20" s="28">
+        <f>[5]gpt_results!G17</f>
+        <v>9.7109585999999998E-2</v>
+      </c>
+      <c r="J20" s="28">
+        <f>[5]gpt_results!H17</f>
+        <v>0.18021390000000001</v>
+      </c>
+      <c r="K20" s="29" t="str">
+        <f>[5]gpt_results!I17</f>
+        <v>joy</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C21" s="31" t="str">
+        <f>[5]gpt_results!A18</f>
+        <v>The constant delays and excuses from the company made me lose my patience.</v>
+      </c>
+      <c r="D21" s="29" t="str">
+        <f>[5]gpt_results!B18</f>
+        <v>anger</v>
+      </c>
+      <c r="E21" s="28">
+        <f>[5]gpt_results!C18</f>
+        <v>0.88482830000000001</v>
+      </c>
+      <c r="F21" s="28">
+        <f>[5]gpt_results!D18</f>
+        <v>4.1374117000000002E-2</v>
+      </c>
+      <c r="G21" s="28">
+        <f>[5]gpt_results!E18</f>
+        <v>1.4967945E-3</v>
+      </c>
+      <c r="H21" s="28">
+        <f>[5]gpt_results!F18</f>
+        <v>2.3871103999999999E-4</v>
+      </c>
+      <c r="I21" s="28">
+        <f>[5]gpt_results!G18</f>
+        <v>7.1745840000000005E-2</v>
+      </c>
+      <c r="J21" s="28">
+        <f>[5]gpt_results!H18</f>
+        <v>3.1624426000000002E-4</v>
+      </c>
+      <c r="K21" s="29" t="str">
+        <f>[5]gpt_results!I18</f>
+        <v>anger</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C22" s="31" t="str">
+        <f>[5]gpt_results!A19</f>
+        <v>Driving through the foggy night, he could barely see a few feet ahead, feeling a chill of fear.</v>
+      </c>
+      <c r="D22" s="29" t="str">
+        <f>[5]gpt_results!B19</f>
+        <v>fear</v>
+      </c>
+      <c r="E22" s="28">
+        <f>[5]gpt_results!C19</f>
+        <v>1.07949E-2</v>
+      </c>
+      <c r="F22" s="28">
+        <f>[5]gpt_results!D19</f>
+        <v>0.98475250000000003</v>
+      </c>
+      <c r="G22" s="28">
+        <f>[5]gpt_results!E19</f>
+        <v>4.7142978000000002E-4</v>
+      </c>
+      <c r="H22" s="28">
+        <f>[5]gpt_results!F19</f>
+        <v>3.5953932E-4</v>
+      </c>
+      <c r="I22" s="28">
+        <f>[5]gpt_results!G19</f>
+        <v>5.1585864000000005E-4</v>
+      </c>
+      <c r="J22" s="28">
+        <f>[5]gpt_results!H19</f>
+        <v>3.1058344000000002E-3</v>
+      </c>
+      <c r="K22" s="29" t="str">
+        <f>[5]gpt_results!I19</f>
+        <v>fear</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C23" s="31" t="str">
+        <f>[5]gpt_results!A20</f>
+        <v>Her face lit up with joy when she saw the beautiful, unexpected gift.</v>
+      </c>
+      <c r="D23" s="29" t="str">
+        <f>[5]gpt_results!B20</f>
+        <v>joy</v>
+      </c>
+      <c r="E23" s="28">
+        <f>[5]gpt_results!C20</f>
+        <v>4.2080745999999998E-6</v>
+      </c>
+      <c r="F23" s="28">
+        <f>[5]gpt_results!D20</f>
+        <v>5.050541E-5</v>
+      </c>
+      <c r="G23" s="28">
+        <f>[5]gpt_results!E20</f>
+        <v>0.99750536999999995</v>
+      </c>
+      <c r="H23" s="28">
+        <f>[5]gpt_results!F20</f>
+        <v>1.4053572999999999E-4</v>
+      </c>
+      <c r="I23" s="28">
+        <f>[5]gpt_results!G20</f>
+        <v>3.7942960000000003E-5</v>
+      </c>
+      <c r="J23" s="28">
+        <f>[5]gpt_results!H20</f>
+        <v>2.2614808E-3</v>
+      </c>
+      <c r="K23" s="29" t="str">
+        <f>[5]gpt_results!I20</f>
+        <v>joy</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C24" s="31" t="str">
+        <f>[5]gpt_results!A21</f>
+        <v>Every day, he made sure to remind her how much he loved her with little gestures and kind words.</v>
+      </c>
+      <c r="D24" s="29" t="str">
+        <f>[5]gpt_results!B21</f>
+        <v>love</v>
+      </c>
+      <c r="E24" s="28">
+        <f>[5]gpt_results!C21</f>
+        <v>1.7888928000000001E-3</v>
+      </c>
+      <c r="F24" s="28">
+        <f>[5]gpt_results!D21</f>
+        <v>3.8236912999999998E-3</v>
+      </c>
+      <c r="G24" s="28">
+        <f>[5]gpt_results!E21</f>
+        <v>0.37963805</v>
+      </c>
+      <c r="H24" s="28">
+        <f>[5]gpt_results!F21</f>
+        <v>0.59053560000000005</v>
+      </c>
+      <c r="I24" s="28">
+        <f>[5]gpt_results!G21</f>
+        <v>2.3350513E-2</v>
+      </c>
+      <c r="J24" s="28">
+        <f>[5]gpt_results!H21</f>
+        <v>8.6324627000000003E-4</v>
+      </c>
+      <c r="K24" s="29" t="str">
+        <f>[5]gpt_results!I21</f>
+        <v>love</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:J1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="7" tint="-0.499984740745262"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K24">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>A5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>